<commit_message>
added comment function, bug fix
</commit_message>
<xml_diff>
--- a/sentences.xlsx
+++ b/sentences.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="162">
   <si>
     <t>Structure</t>
   </si>
@@ -222,9 +222,6 @@
     <t xml:space="preserve"> - educated(X) :- ...</t>
   </si>
   <si>
-    <t xml:space="preserve"> :- ...</t>
-  </si>
-  <si>
     <t>... :- person(roberta).</t>
   </si>
   <si>
@@ -247,9 +244,6 @@
   </si>
   <si>
     <t>... :- not tall(roberta).</t>
-  </si>
-  <si>
-    <t>... :-</t>
   </si>
   <si>
     <t>Variable is Adjective.</t>
@@ -558,6 +552,147 @@
   </si>
   <si>
     <t>... :- not work_for(roberta, X), person(X).</t>
+  </si>
+  <si>
+    <t>pNounVerbACNounAsPNoun</t>
+  </si>
+  <si>
+    <t>[a] PNoun Verb a CNoun as [a] Pnoun.</t>
+  </si>
+  <si>
+    <t>[a] Pnoun not Verb a CNoun as [a] Pnoun.</t>
+  </si>
+  <si>
+    <t>Roberta holds a job as a nurse.</t>
+  </si>
+  <si>
+    <t>Roberta does not hold a job as a nurse.</t>
+  </si>
+  <si>
+    <r>
+      <t>.* a .* as .*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+      </rPr>
+      <t>\\</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+      </rPr>
+      <t>.$</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> - hold(roberta, nurse) :- ...</t>
+  </si>
+  <si>
+    <t>hold(roberta, nurse) :- ...</t>
+  </si>
+  <si>
+    <t>... :- hold(roberta, nurse), job(nurse).</t>
+  </si>
+  <si>
+    <t>... :- not hold(roberta, nurse), job(nurse).</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">there is(n't | n't | not | )a .* [a-z] </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+      </rPr>
+      <t>\\</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+      </rPr>
+      <t>.$</t>
+    </r>
+  </si>
+  <si>
+    <t>thereIsACNounVariable</t>
+  </si>
+  <si>
+    <t>there is a CNoun Variable.</t>
+  </si>
+  <si>
+    <t>there is not a CNoun Variable.</t>
+  </si>
+  <si>
+    <t>There is a person X.</t>
+  </si>
+  <si>
+    <t>There is not a person X.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - person(X) :- ...</t>
+  </si>
+  <si>
+    <t>... :- not person(X).</t>
+  </si>
+  <si>
+    <t>... :- person(X).</t>
+  </si>
+  <si>
+    <t>... :- #count{Y : hold(X, Y)} &gt; 2.</t>
+  </si>
+  <si>
+    <t>cNounVariableVerbMoreLessThanNumberCNounVariable</t>
+  </si>
+  <si>
+    <r>
+      <t>.* (more|less) than .*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+      </rPr>
+      <t>\\</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+      </rPr>
+      <t>.$</t>
+    </r>
+  </si>
+  <si>
+    <t>CNoun Variable Verb more than Number CNoun Variable.</t>
+  </si>
+  <si>
+    <t>CNoun Variable Verb less than Number CNoun Variable.</t>
+  </si>
+  <si>
+    <t>Person X holds more than two jobs Y.</t>
+  </si>
+  <si>
+    <t>... :- #count{Y : hold(X, Y)} &lt; 2.</t>
+  </si>
+  <si>
+    <t>Person X holds less than two jobs Y.</t>
   </si>
 </sst>
 </file>
@@ -642,8 +777,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -691,7 +832,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -710,6 +851,9 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -728,6 +872,9 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1003,18 +1150,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H31"/>
+  <dimension ref="A3:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="34.6640625" bestFit="1" customWidth="1"/>
@@ -1064,10 +1211,10 @@
         <v>9</v>
       </c>
       <c r="G4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1090,10 +1237,10 @@
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1208,10 +1355,10 @@
         <v>15</v>
       </c>
       <c r="G10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -1234,10 +1381,10 @@
         <v>17</v>
       </c>
       <c r="G11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -1245,7 +1392,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>12</v>
@@ -1254,13 +1401,13 @@
         <v>13</v>
       </c>
       <c r="E12" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" t="s">
         <v>63</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>65</v>
-      </c>
-      <c r="H12" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -1268,7 +1415,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>12</v>
@@ -1277,13 +1424,13 @@
         <v>13</v>
       </c>
       <c r="E13" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" t="s">
         <v>64</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>66</v>
-      </c>
-      <c r="H13" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
@@ -1336,46 +1483,46 @@
       <c r="A16">
         <v>13</v>
       </c>
-      <c r="B16" t="s">
-        <v>73</v>
+      <c r="B16" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>70</v>
+        <v>140</v>
       </c>
       <c r="D16" t="s">
-        <v>75</v>
+        <v>135</v>
       </c>
       <c r="E16" t="s">
-        <v>69</v>
+        <v>138</v>
       </c>
       <c r="G16" t="s">
-        <v>71</v>
+        <v>143</v>
       </c>
       <c r="H16" t="s">
-        <v>72</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>14</v>
       </c>
-      <c r="B17" t="s">
-        <v>74</v>
+      <c r="B17" s="2" t="s">
+        <v>137</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>70</v>
+        <v>140</v>
       </c>
       <c r="D17" t="s">
-        <v>75</v>
+        <v>135</v>
       </c>
       <c r="E17" t="s">
-        <v>76</v>
+        <v>139</v>
       </c>
       <c r="G17" t="s">
-        <v>80</v>
+        <v>144</v>
       </c>
       <c r="H17" t="s">
-        <v>77</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -1383,22 +1530,22 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>121</v>
+        <v>71</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="D18" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E18" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="G18" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="H18" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -1406,68 +1553,68 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="D19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" t="s">
+        <v>74</v>
+      </c>
+      <c r="G19" t="s">
         <v>78</v>
       </c>
-      <c r="E19" t="s">
-        <v>87</v>
-      </c>
-      <c r="G19" t="s">
-        <v>82</v>
-      </c>
       <c r="H19" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>17</v>
       </c>
-      <c r="B20" t="s">
-        <v>120</v>
+      <c r="B20" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" t="s">
+        <v>76</v>
+      </c>
+      <c r="E20" t="s">
+        <v>86</v>
+      </c>
+      <c r="G20" t="s">
         <v>79</v>
       </c>
-      <c r="D20" t="s">
-        <v>78</v>
-      </c>
-      <c r="E20" t="s">
-        <v>122</v>
-      </c>
-      <c r="G20" t="s">
-        <v>127</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>124</v>
+      <c r="H20" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>18</v>
       </c>
-      <c r="B21" t="s">
-        <v>119</v>
+      <c r="B21" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E21" t="s">
-        <v>123</v>
+        <v>85</v>
       </c>
       <c r="G21" t="s">
-        <v>126</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>125</v>
+        <v>80</v>
+      </c>
+      <c r="H21" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1475,22 +1622,22 @@
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="D22" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="E22" t="s">
-        <v>89</v>
+        <v>120</v>
       </c>
       <c r="G22" t="s">
-        <v>86</v>
+        <v>125</v>
       </c>
       <c r="H22" t="s">
-        <v>90</v>
+        <v>122</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -1498,22 +1645,22 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="D23" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="E23" t="s">
-        <v>94</v>
+        <v>121</v>
       </c>
       <c r="G23" t="s">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="H23" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -1521,97 +1668,91 @@
         <v>21</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>129</v>
+        <v>90</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D24" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E24" t="s">
-        <v>131</v>
+        <v>87</v>
       </c>
       <c r="G24" t="s">
-        <v>135</v>
+        <v>84</v>
       </c>
       <c r="H24" t="s">
-        <v>133</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>22</v>
       </c>
-      <c r="B25" t="s">
-        <v>130</v>
+      <c r="B25" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D25" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" t="s">
+        <v>92</v>
+      </c>
+      <c r="G25" t="s">
         <v>93</v>
       </c>
-      <c r="D25" t="s">
-        <v>91</v>
-      </c>
-      <c r="E25" t="s">
-        <v>132</v>
-      </c>
-      <c r="G25" t="s">
-        <v>136</v>
-      </c>
       <c r="H25" t="s">
-        <v>134</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>23</v>
       </c>
-      <c r="B26" t="s">
-        <v>98</v>
+      <c r="B26" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D26" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="E26" t="s">
-        <v>102</v>
-      </c>
-      <c r="F26" t="s">
-        <v>104</v>
+        <v>129</v>
       </c>
       <c r="G26" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="H26" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>24</v>
       </c>
-      <c r="B27" t="s">
-        <v>99</v>
+      <c r="B27" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D27" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="E27" t="s">
-        <v>103</v>
-      </c>
-      <c r="F27" t="s">
-        <v>107</v>
+        <v>130</v>
       </c>
       <c r="G27" t="s">
-        <v>108</v>
+        <v>134</v>
       </c>
       <c r="H27" t="s">
-        <v>109</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -1619,25 +1760,25 @@
         <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D28" t="s">
+        <v>99</v>
+      </c>
+      <c r="E28" t="s">
         <v>100</v>
       </c>
-      <c r="D28" t="s">
-        <v>101</v>
-      </c>
-      <c r="E28" t="s">
-        <v>110</v>
-      </c>
       <c r="F28" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="G28" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="H28" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -1645,41 +1786,157 @@
         <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D29" t="s">
+        <v>99</v>
+      </c>
+      <c r="E29" t="s">
         <v>101</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
+        <v>105</v>
+      </c>
+      <c r="G29" t="s">
+        <v>106</v>
+      </c>
+      <c r="H29" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>27</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D30" t="s">
+        <v>99</v>
+      </c>
+      <c r="E30" t="s">
+        <v>108</v>
+      </c>
+      <c r="F30" t="s">
+        <v>109</v>
+      </c>
+      <c r="G30" t="s">
+        <v>110</v>
+      </c>
+      <c r="H30" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>28</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F29" t="s">
+      <c r="C31" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" t="s">
+        <v>99</v>
+      </c>
+      <c r="E31" t="s">
         <v>114</v>
       </c>
-      <c r="G29" t="s">
-        <v>115</v>
-      </c>
-      <c r="H29" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G30" t="s">
-        <v>60</v>
-      </c>
-      <c r="H30" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F31" t="s">
+        <v>112</v>
+      </c>
       <c r="G31" t="s">
-        <v>60</v>
+        <v>113</v>
       </c>
       <c r="H31" t="s">
-        <v>51</v>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>29</v>
+      </c>
+      <c r="B32" t="s">
+        <v>147</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D32" t="s">
+        <v>146</v>
+      </c>
+      <c r="E32" t="s">
+        <v>149</v>
+      </c>
+      <c r="G32" t="s">
+        <v>153</v>
+      </c>
+      <c r="H32" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>30</v>
+      </c>
+      <c r="B33" t="s">
+        <v>148</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D33" t="s">
+        <v>146</v>
+      </c>
+      <c r="E33" t="s">
+        <v>150</v>
+      </c>
+      <c r="G33" t="s">
+        <v>152</v>
+      </c>
+      <c r="H33" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B34" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D34" t="s">
+        <v>155</v>
+      </c>
+      <c r="E34" t="s">
+        <v>159</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B35" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D35" t="s">
+        <v>155</v>
+      </c>
+      <c r="E35" t="s">
+        <v>161</v>
+      </c>
+      <c r="G35" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added open file function
</commit_message>
<xml_diff>
--- a/sentences.xlsx
+++ b/sentences.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="172">
   <si>
     <t>Structure</t>
   </si>
@@ -693,6 +693,56 @@
   </si>
   <si>
     <t>Person X holds less than two jobs Y.</t>
+  </si>
+  <si>
+    <r>
+      <t>a .* is(n't | n't | not | )a .* of a .*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+      </rPr>
+      <t>\\</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>aCNounVariableIsACNounOfACNounVariable</t>
+  </si>
+  <si>
+    <t>a CNoun Variable is a CNoun of a Cnoun Variable.</t>
+  </si>
+  <si>
+    <t>a CNoun Variable is not a CNoun of a CNoun Variable.</t>
+  </si>
+  <si>
+    <t>husband(X, Y) :- ...</t>
+  </si>
+  <si>
+    <t>A person X is a husband of a person Y.</t>
+  </si>
+  <si>
+    <t>A person X is not a husband of a person Y.</t>
+  </si>
+  <si>
+    <t>... :- not husband(X, Y), person(X), person(Y).</t>
+  </si>
+  <si>
+    <t>... :- husband(X, Y), person(X), person(Y).</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - husband(X, Y) :- ...</t>
   </si>
 </sst>
 </file>
@@ -777,8 +827,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -832,7 +884,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -854,6 +906,7 @@
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -875,6 +928,7 @@
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1150,10 +1204,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H35"/>
+  <dimension ref="A3:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1162,9 +1216,9 @@
     <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1886,7 +1940,7 @@
       <c r="A33">
         <v>30</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="2" t="s">
         <v>148</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -1906,6 +1960,9 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>31</v>
+      </c>
       <c r="B34" s="2" t="s">
         <v>157</v>
       </c>
@@ -1923,6 +1980,9 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>32</v>
+      </c>
       <c r="B35" s="2" t="s">
         <v>158</v>
       </c>
@@ -1938,6 +1998,64 @@
       <c r="G35" t="s">
         <v>160</v>
       </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>33</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D36" t="s">
+        <v>163</v>
+      </c>
+      <c r="E36" t="s">
+        <v>167</v>
+      </c>
+      <c r="G36" t="s">
+        <v>170</v>
+      </c>
+      <c r="H36" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>34</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D37" t="s">
+        <v>163</v>
+      </c>
+      <c r="E37" t="s">
+        <v>168</v>
+      </c>
+      <c r="G37" t="s">
+        <v>169</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B38" s="2"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B39" s="2"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B40" s="2"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B41" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added "PNoun is adjective preposition"
</commit_message>
<xml_diff>
--- a/sentences.xlsx
+++ b/sentences.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="193">
   <si>
     <t>Structure</t>
   </si>
@@ -743,6 +743,69 @@
   </si>
   <si>
     <t xml:space="preserve"> - husband(X, Y) :- ...</t>
+  </si>
+  <si>
+    <t>PNoun is Adjective Preposition Pnoun</t>
+  </si>
+  <si>
+    <t>PNoun is Preposition Pnoun</t>
+  </si>
+  <si>
+    <t>PNoun is not Preposition Pnoun</t>
+  </si>
+  <si>
+    <t>Roberta is at work.</t>
+  </si>
+  <si>
+    <t>Roberta is not at work.</t>
+  </si>
+  <si>
+    <t>pNounIsAdjectivePrepositionPNoun</t>
+  </si>
+  <si>
+    <t>at(roberta, work).</t>
+  </si>
+  <si>
+    <t>... :- at(roberta, work).</t>
+  </si>
+  <si>
+    <t>... :- not at(roberta, work).</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - at(roberta, work).</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - at(roberta, work) :- ...</t>
+  </si>
+  <si>
+    <t>at(roberta, work) :- ...</t>
+  </si>
+  <si>
+    <t>PNoun is not Adjective Preposition Pnoun</t>
+  </si>
+  <si>
+    <t>Roberta is married to bob.</t>
+  </si>
+  <si>
+    <t>Roberta is not married to bob.</t>
+  </si>
+  <si>
+    <t>married_to(roberta, bob).</t>
+  </si>
+  <si>
+    <t>... :- married_to(roberta, bob).</t>
+  </si>
+  <si>
+    <t>... :- not married_to(roberta, bob).</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - married_to(roberta, bob).</t>
+  </si>
+  <si>
+    <t>married_to(roberta, bob) :- ...</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - married_to(roberta, bob) :- ...</t>
   </si>
 </sst>
 </file>
@@ -827,8 +890,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="45">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -884,7 +959,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="57">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -907,6 +982,12 @@
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -929,6 +1010,12 @@
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1204,10 +1291,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H41"/>
+  <dimension ref="A3:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A8" zoomScale="168" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1217,9 +1304,9 @@
     <col min="3" max="3" width="39.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="38" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -1534,528 +1621,620 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>13</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>136</v>
+      <c r="B16" t="s">
+        <v>173</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>140</v>
+        <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>135</v>
+        <v>177</v>
       </c>
       <c r="E16" t="s">
-        <v>138</v>
+        <v>175</v>
+      </c>
+      <c r="F16" t="s">
+        <v>178</v>
       </c>
       <c r="G16" t="s">
-        <v>143</v>
+        <v>179</v>
       </c>
       <c r="H16" t="s">
-        <v>142</v>
+        <v>183</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>14</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>137</v>
+      <c r="B17" t="s">
+        <v>174</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>140</v>
+        <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>135</v>
+        <v>177</v>
       </c>
       <c r="E17" t="s">
-        <v>139</v>
+        <v>176</v>
+      </c>
+      <c r="F17" t="s">
+        <v>181</v>
       </c>
       <c r="G17" t="s">
-        <v>144</v>
+        <v>180</v>
       </c>
       <c r="H17" t="s">
-        <v>141</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>15</v>
-      </c>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>172</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>73</v>
+        <v>177</v>
       </c>
       <c r="E18" t="s">
-        <v>67</v>
+        <v>185</v>
+      </c>
+      <c r="F18" t="s">
+        <v>187</v>
       </c>
       <c r="G18" t="s">
-        <v>69</v>
+        <v>188</v>
       </c>
       <c r="H18" t="s">
-        <v>70</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>16</v>
-      </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>184</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>73</v>
+        <v>177</v>
       </c>
       <c r="E19" t="s">
-        <v>74</v>
+        <v>186</v>
+      </c>
+      <c r="F19" t="s">
+        <v>190</v>
       </c>
       <c r="G19" t="s">
-        <v>78</v>
+        <v>189</v>
       </c>
       <c r="H19" t="s">
-        <v>75</v>
+        <v>192</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>77</v>
+        <v>140</v>
       </c>
       <c r="D20" t="s">
-        <v>76</v>
+        <v>135</v>
       </c>
       <c r="E20" t="s">
-        <v>86</v>
+        <v>138</v>
       </c>
       <c r="G20" t="s">
-        <v>79</v>
+        <v>143</v>
       </c>
       <c r="H20" t="s">
-        <v>81</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>83</v>
+        <v>137</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>77</v>
+        <v>140</v>
       </c>
       <c r="D21" t="s">
-        <v>76</v>
+        <v>135</v>
       </c>
       <c r="E21" t="s">
-        <v>85</v>
+        <v>139</v>
       </c>
       <c r="G21" t="s">
-        <v>80</v>
+        <v>144</v>
       </c>
       <c r="H21" t="s">
-        <v>82</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>118</v>
+        <v>71</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D22" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E22" t="s">
-        <v>120</v>
+        <v>67</v>
       </c>
       <c r="G22" t="s">
-        <v>125</v>
+        <v>69</v>
       </c>
       <c r="H22" t="s">
-        <v>122</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>117</v>
+        <v>72</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D23" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E23" t="s">
-        <v>121</v>
+        <v>74</v>
       </c>
       <c r="G23" t="s">
-        <v>124</v>
+        <v>78</v>
       </c>
       <c r="H23" t="s">
-        <v>123</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>90</v>
+        <v>119</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G24" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H24" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D25" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E25" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G25" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="H25" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>23</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>127</v>
+        <v>19</v>
+      </c>
+      <c r="B26" t="s">
+        <v>118</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D26" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E26" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="G26" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="H26" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>24</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>128</v>
+        <v>20</v>
+      </c>
+      <c r="B27" t="s">
+        <v>117</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D27" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E27" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="G27" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="H27" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>25</v>
-      </c>
-      <c r="B28" t="s">
-        <v>96</v>
+        <v>21</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D28" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="E28" t="s">
-        <v>100</v>
-      </c>
-      <c r="F28" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="G28" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="H28" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>26</v>
-      </c>
-      <c r="B29" t="s">
-        <v>97</v>
+        <v>22</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D29" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="E29" t="s">
-        <v>101</v>
-      </c>
-      <c r="F29" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="G29" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="H29" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D30" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="E30" t="s">
-        <v>108</v>
-      </c>
-      <c r="F30" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="G30" t="s">
-        <v>110</v>
+        <v>133</v>
       </c>
       <c r="H30" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D31" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="E31" t="s">
-        <v>114</v>
-      </c>
-      <c r="F31" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="G31" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="H31" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B32" t="s">
-        <v>147</v>
+        <v>96</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>145</v>
+        <v>98</v>
       </c>
       <c r="D32" t="s">
-        <v>146</v>
+        <v>99</v>
       </c>
       <c r="E32" t="s">
-        <v>149</v>
+        <v>100</v>
+      </c>
+      <c r="F32" t="s">
+        <v>102</v>
       </c>
       <c r="G32" t="s">
-        <v>153</v>
+        <v>103</v>
       </c>
       <c r="H32" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>30</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>148</v>
+        <v>26</v>
+      </c>
+      <c r="B33" t="s">
+        <v>97</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>145</v>
+        <v>98</v>
       </c>
       <c r="D33" t="s">
-        <v>146</v>
+        <v>99</v>
       </c>
       <c r="E33" t="s">
-        <v>150</v>
+        <v>101</v>
+      </c>
+      <c r="F33" t="s">
+        <v>105</v>
       </c>
       <c r="G33" t="s">
-        <v>152</v>
+        <v>106</v>
       </c>
       <c r="H33" t="s">
-        <v>151</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>157</v>
+        <v>115</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>156</v>
+        <v>98</v>
       </c>
       <c r="D34" t="s">
-        <v>155</v>
+        <v>99</v>
       </c>
       <c r="E34" t="s">
-        <v>159</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>154</v>
+        <v>108</v>
+      </c>
+      <c r="F34" t="s">
+        <v>109</v>
+      </c>
+      <c r="G34" t="s">
+        <v>110</v>
+      </c>
+      <c r="H34" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>158</v>
+        <v>116</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>156</v>
+        <v>98</v>
       </c>
       <c r="D35" t="s">
-        <v>155</v>
+        <v>99</v>
       </c>
       <c r="E35" t="s">
-        <v>161</v>
+        <v>114</v>
+      </c>
+      <c r="F35" t="s">
+        <v>112</v>
       </c>
       <c r="G35" t="s">
-        <v>160</v>
+        <v>113</v>
+      </c>
+      <c r="H35" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>33</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>164</v>
+        <v>29</v>
+      </c>
+      <c r="B36" t="s">
+        <v>147</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="D36" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="E36" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="G36" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="H36" t="s">
-        <v>166</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37">
+        <v>30</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D37" t="s">
+        <v>146</v>
+      </c>
+      <c r="E37" t="s">
+        <v>150</v>
+      </c>
+      <c r="G37" t="s">
+        <v>152</v>
+      </c>
+      <c r="H37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>31</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D38" t="s">
+        <v>155</v>
+      </c>
+      <c r="E38" t="s">
+        <v>159</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>32</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D39" t="s">
+        <v>155</v>
+      </c>
+      <c r="E39" t="s">
+        <v>161</v>
+      </c>
+      <c r="G39" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>33</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D40" t="s">
+        <v>163</v>
+      </c>
+      <c r="E40" t="s">
+        <v>167</v>
+      </c>
+      <c r="G40" t="s">
+        <v>170</v>
+      </c>
+      <c r="H40" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41">
         <v>34</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D41" t="s">
         <v>163</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E41" t="s">
         <v>168</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G41" t="s">
         <v>169</v>
       </c>
-      <c r="H37" s="5" t="s">
+      <c r="H41" s="5" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B38" s="2"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B39" s="2"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B40" s="2"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B41" s="2"/>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B42" s="2"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B43" s="2"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B44" s="2"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B45" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added "PNoun is Adjective Preposition CNoun Variable"
</commit_message>
<xml_diff>
--- a/sentences.xlsx
+++ b/sentences.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="201">
   <si>
     <t>Structure</t>
   </si>
@@ -745,15 +745,6 @@
     <t xml:space="preserve"> - husband(X, Y) :- ...</t>
   </si>
   <si>
-    <t>PNoun is Adjective Preposition Pnoun</t>
-  </si>
-  <si>
-    <t>PNoun is Preposition Pnoun</t>
-  </si>
-  <si>
-    <t>PNoun is not Preposition Pnoun</t>
-  </si>
-  <si>
     <t>Roberta is at work.</t>
   </si>
   <si>
@@ -781,9 +772,6 @@
     <t>at(roberta, work) :- ...</t>
   </si>
   <si>
-    <t>PNoun is not Adjective Preposition Pnoun</t>
-  </si>
-  <si>
     <t>Roberta is married to bob.</t>
   </si>
   <si>
@@ -806,6 +794,42 @@
   </si>
   <si>
     <t xml:space="preserve"> - married_to(roberta, bob) :- ...</t>
+  </si>
+  <si>
+    <t>PNoun is Preposition Pnoun.</t>
+  </si>
+  <si>
+    <t>PNoun is not Preposition Pnoun.</t>
+  </si>
+  <si>
+    <t>PNoun is Adjective Preposition Pnoun.</t>
+  </si>
+  <si>
+    <t>PNoun is not Adjective Preposition Pnoun.</t>
+  </si>
+  <si>
+    <t>CNoun Variable is Preposition Pnoun.</t>
+  </si>
+  <si>
+    <t>CNoun Variable is not Preposition Pnoun.</t>
+  </si>
+  <si>
+    <t>CNoun Variable is Adjective Preposition Pnoun.</t>
+  </si>
+  <si>
+    <t>CNoun Variable is not Adjective Preposition Pnoun.</t>
+  </si>
+  <si>
+    <t>Person X is at work.</t>
+  </si>
+  <si>
+    <t>Person X is not at work.</t>
+  </si>
+  <si>
+    <t>Person X is married to bob.</t>
+  </si>
+  <si>
+    <t>Person X is not married to bob.</t>
   </si>
 </sst>
 </file>
@@ -890,8 +914,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -959,7 +985,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="57">
+  <cellStyles count="59">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -988,6 +1014,7 @@
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1016,6 +1043,7 @@
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1291,10 +1319,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H45"/>
+  <dimension ref="A3:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A8" zoomScale="168" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A9" zoomScale="168" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1622,619 +1650,663 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E16" t="s">
+        <v>172</v>
+      </c>
+      <c r="F16" t="s">
         <v>175</v>
       </c>
-      <c r="F16" t="s">
-        <v>178</v>
-      </c>
       <c r="G16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H16" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>174</v>
+        <v>190</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D17" t="s">
+        <v>174</v>
+      </c>
+      <c r="E17" t="s">
+        <v>173</v>
+      </c>
+      <c r="F17" t="s">
+        <v>178</v>
+      </c>
+      <c r="G17" t="s">
         <v>177</v>
       </c>
-      <c r="E17" t="s">
-        <v>176</v>
-      </c>
-      <c r="F17" t="s">
-        <v>181</v>
-      </c>
-      <c r="G17" t="s">
-        <v>180</v>
-      </c>
       <c r="H17" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E18" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="F18" t="s">
+        <v>183</v>
+      </c>
+      <c r="G18" t="s">
+        <v>184</v>
+      </c>
+      <c r="H18" t="s">
         <v>187</v>
-      </c>
-      <c r="G18" t="s">
-        <v>188</v>
-      </c>
-      <c r="H18" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E19" t="s">
+        <v>182</v>
+      </c>
+      <c r="F19" t="s">
         <v>186</v>
       </c>
-      <c r="F19" t="s">
-        <v>190</v>
-      </c>
       <c r="G19" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="H19" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>13</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>136</v>
+      <c r="B20" t="s">
+        <v>193</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D20" t="s">
-        <v>135</v>
+        <v>28</v>
       </c>
       <c r="E20" t="s">
-        <v>138</v>
-      </c>
-      <c r="G20" t="s">
-        <v>143</v>
-      </c>
-      <c r="H20" t="s">
-        <v>142</v>
+        <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>14</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>137</v>
+      <c r="B21" t="s">
+        <v>194</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D21" t="s">
-        <v>135</v>
+        <v>28</v>
       </c>
       <c r="E21" t="s">
-        <v>139</v>
-      </c>
-      <c r="G21" t="s">
-        <v>144</v>
-      </c>
-      <c r="H21" t="s">
-        <v>141</v>
+        <v>198</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>15</v>
-      </c>
       <c r="B22" t="s">
-        <v>71</v>
+        <v>195</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
       <c r="E22" t="s">
-        <v>67</v>
-      </c>
-      <c r="G22" t="s">
-        <v>69</v>
-      </c>
-      <c r="H22" t="s">
-        <v>70</v>
+        <v>199</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>16</v>
-      </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>196</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
       <c r="E23" t="s">
-        <v>74</v>
-      </c>
-      <c r="G23" t="s">
-        <v>78</v>
-      </c>
-      <c r="H23" t="s">
-        <v>75</v>
+        <v>200</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>77</v>
+        <v>140</v>
       </c>
       <c r="D24" t="s">
-        <v>76</v>
+        <v>135</v>
       </c>
       <c r="E24" t="s">
-        <v>86</v>
+        <v>138</v>
       </c>
       <c r="G24" t="s">
-        <v>79</v>
+        <v>143</v>
       </c>
       <c r="H24" t="s">
-        <v>81</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>83</v>
+        <v>137</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>77</v>
+        <v>140</v>
       </c>
       <c r="D25" t="s">
-        <v>76</v>
+        <v>135</v>
       </c>
       <c r="E25" t="s">
-        <v>85</v>
+        <v>139</v>
       </c>
       <c r="G25" t="s">
-        <v>80</v>
+        <v>144</v>
       </c>
       <c r="H25" t="s">
-        <v>82</v>
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>118</v>
+        <v>71</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D26" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E26" t="s">
-        <v>120</v>
+        <v>67</v>
       </c>
       <c r="G26" t="s">
-        <v>125</v>
+        <v>69</v>
       </c>
       <c r="H26" t="s">
-        <v>122</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>117</v>
+        <v>72</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D27" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E27" t="s">
-        <v>121</v>
+        <v>74</v>
       </c>
       <c r="G27" t="s">
-        <v>124</v>
+        <v>78</v>
       </c>
       <c r="H27" t="s">
-        <v>123</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>90</v>
+        <v>119</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D28" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G28" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H28" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D29" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E29" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G29" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="H29" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>23</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>127</v>
+        <v>19</v>
+      </c>
+      <c r="B30" t="s">
+        <v>118</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D30" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E30" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="G30" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="H30" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>24</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>128</v>
+        <v>20</v>
+      </c>
+      <c r="B31" t="s">
+        <v>117</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D31" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E31" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="G31" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="H31" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>25</v>
-      </c>
-      <c r="B32" t="s">
-        <v>96</v>
+        <v>21</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D32" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="E32" t="s">
-        <v>100</v>
-      </c>
-      <c r="F32" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="G32" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="H32" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>26</v>
-      </c>
-      <c r="B33" t="s">
-        <v>97</v>
+        <v>22</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D33" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="E33" t="s">
-        <v>101</v>
-      </c>
-      <c r="F33" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="G33" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="H33" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D34" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="E34" t="s">
-        <v>108</v>
-      </c>
-      <c r="F34" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="G34" t="s">
-        <v>110</v>
+        <v>133</v>
       </c>
       <c r="H34" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D35" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="E35" t="s">
-        <v>114</v>
-      </c>
-      <c r="F35" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="G35" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="H35" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B36" t="s">
-        <v>147</v>
+        <v>96</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>145</v>
+        <v>98</v>
       </c>
       <c r="D36" t="s">
-        <v>146</v>
+        <v>99</v>
       </c>
       <c r="E36" t="s">
-        <v>149</v>
+        <v>100</v>
+      </c>
+      <c r="F36" t="s">
+        <v>102</v>
       </c>
       <c r="G36" t="s">
-        <v>153</v>
+        <v>103</v>
       </c>
       <c r="H36" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>30</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>148</v>
+        <v>26</v>
+      </c>
+      <c r="B37" t="s">
+        <v>97</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>145</v>
+        <v>98</v>
       </c>
       <c r="D37" t="s">
-        <v>146</v>
+        <v>99</v>
       </c>
       <c r="E37" t="s">
-        <v>150</v>
+        <v>101</v>
+      </c>
+      <c r="F37" t="s">
+        <v>105</v>
       </c>
       <c r="G37" t="s">
-        <v>152</v>
+        <v>106</v>
       </c>
       <c r="H37" t="s">
-        <v>151</v>
+        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>157</v>
+        <v>115</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>156</v>
+        <v>98</v>
       </c>
       <c r="D38" t="s">
-        <v>155</v>
+        <v>99</v>
       </c>
       <c r="E38" t="s">
-        <v>159</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>154</v>
+        <v>108</v>
+      </c>
+      <c r="F38" t="s">
+        <v>109</v>
+      </c>
+      <c r="G38" t="s">
+        <v>110</v>
+      </c>
+      <c r="H38" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>158</v>
+        <v>116</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>156</v>
+        <v>98</v>
       </c>
       <c r="D39" t="s">
-        <v>155</v>
+        <v>99</v>
       </c>
       <c r="E39" t="s">
-        <v>161</v>
+        <v>114</v>
+      </c>
+      <c r="F39" t="s">
+        <v>112</v>
       </c>
       <c r="G39" t="s">
-        <v>160</v>
+        <v>113</v>
+      </c>
+      <c r="H39" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>33</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>164</v>
+        <v>29</v>
+      </c>
+      <c r="B40" t="s">
+        <v>147</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="D40" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="E40" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="G40" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="H40" t="s">
-        <v>166</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41">
+        <v>30</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D41" t="s">
+        <v>146</v>
+      </c>
+      <c r="E41" t="s">
+        <v>150</v>
+      </c>
+      <c r="G41" t="s">
+        <v>152</v>
+      </c>
+      <c r="H41" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>31</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D42" t="s">
+        <v>155</v>
+      </c>
+      <c r="E42" t="s">
+        <v>159</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>32</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D43" t="s">
+        <v>155</v>
+      </c>
+      <c r="E43" t="s">
+        <v>161</v>
+      </c>
+      <c r="G43" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>33</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D44" t="s">
+        <v>163</v>
+      </c>
+      <c r="E44" t="s">
+        <v>167</v>
+      </c>
+      <c r="G44" t="s">
+        <v>170</v>
+      </c>
+      <c r="H44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45">
         <v>34</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B45" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D45" t="s">
         <v>163</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E45" t="s">
         <v>168</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G45" t="s">
         <v>169</v>
       </c>
-      <c r="H41" s="5" t="s">
+      <c r="H45" s="5" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B42" s="2"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B43" s="2"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B44" s="2"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B45" s="2"/>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B46" s="2"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B47" s="2"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B48" s="2"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B49" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added "CNoun Variable Is Adjective Preposition CNoun VariableIs"
</commit_message>
<xml_diff>
--- a/sentences.xlsx
+++ b/sentences.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="238">
   <si>
     <t>Structure</t>
   </si>
@@ -796,30 +796,6 @@
     <t xml:space="preserve"> - married_to(roberta, bob) :- ...</t>
   </si>
   <si>
-    <t>PNoun is Preposition Pnoun.</t>
-  </si>
-  <si>
-    <t>PNoun is not Preposition Pnoun.</t>
-  </si>
-  <si>
-    <t>PNoun is Adjective Preposition Pnoun.</t>
-  </si>
-  <si>
-    <t>PNoun is not Adjective Preposition Pnoun.</t>
-  </si>
-  <si>
-    <t>CNoun Variable is Preposition Pnoun.</t>
-  </si>
-  <si>
-    <t>CNoun Variable is not Preposition Pnoun.</t>
-  </si>
-  <si>
-    <t>CNoun Variable is Adjective Preposition Pnoun.</t>
-  </si>
-  <si>
-    <t>CNoun Variable is not Adjective Preposition Pnoun.</t>
-  </si>
-  <si>
     <t>Person X is at work.</t>
   </si>
   <si>
@@ -830,6 +806,141 @@
   </si>
   <si>
     <t>Person X is not married to bob.</t>
+  </si>
+  <si>
+    <t>cNounVariableIsAdjectivePrepositionPNoun</t>
+  </si>
+  <si>
+    <t>married_to(X, bob) :- ...</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - married_to(X, bob) :- ...</t>
+  </si>
+  <si>
+    <t>... :- married_to(X, bob), person(X).</t>
+  </si>
+  <si>
+    <t>... :- not married_to(X, bob), person(X).</t>
+  </si>
+  <si>
+    <t>at(X, work) :- ...</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - at(X, work) :- ...</t>
+  </si>
+  <si>
+    <t>... :- at(X, work), person(X).</t>
+  </si>
+  <si>
+    <t>... :- not at(X, work), person(X).</t>
+  </si>
+  <si>
+    <t>CNoun Variable is Preposition CNoun Variable.</t>
+  </si>
+  <si>
+    <t>PNoun is Preposition PNoun.</t>
+  </si>
+  <si>
+    <t>PNoun is not Preposition PNoun.</t>
+  </si>
+  <si>
+    <t>PNoun is Adjective Preposition PNoun.</t>
+  </si>
+  <si>
+    <t>PNoun is not Adjective Preposition PNoun.</t>
+  </si>
+  <si>
+    <t>CNoun Variable is Preposition PNoun.</t>
+  </si>
+  <si>
+    <t>CNoun Variable is not Preposition PNoun.</t>
+  </si>
+  <si>
+    <t>CNoun Variable is Adjective Preposition PNoun.</t>
+  </si>
+  <si>
+    <t>CNoun Variable is not Adjective Preposition PNoun.</t>
+  </si>
+  <si>
+    <t>CNoun Variable is not Preposition CNoun Variable.</t>
+  </si>
+  <si>
+    <t>CNoun Variable is Adjective Preposition CNoun Variable.</t>
+  </si>
+  <si>
+    <t>CNoun Variable is not Adjective Preposition CNoun Variable.</t>
+  </si>
+  <si>
+    <t>PNoun is Preposition CNoun Variable.</t>
+  </si>
+  <si>
+    <t>PNoun is not Preposition CNoun Variable.</t>
+  </si>
+  <si>
+    <t>PNoun is Adjective Preposition CNoun Variable.</t>
+  </si>
+  <si>
+    <t>PNoun is not Adjective Preposition CNoun Variable.</t>
+  </si>
+  <si>
+    <t>.* is(n't | n't | not | ).* [a-z] \\.$</t>
+  </si>
+  <si>
+    <t>Roberta is married to person X.</t>
+  </si>
+  <si>
+    <t>Roberta is not married to person X.</t>
+  </si>
+  <si>
+    <t>Roberta is in room X.</t>
+  </si>
+  <si>
+    <t>Roberta is not in room X.</t>
+  </si>
+  <si>
+    <t>in(roberta, X) :- ...</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - in(roberta, X) :- ...</t>
+  </si>
+  <si>
+    <t>married_to(roberta, X) :- ...</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - married_to(roberta, X) :- ...</t>
+  </si>
+  <si>
+    <t>... :- in(roberta, X), room(X).</t>
+  </si>
+  <si>
+    <t>... :- not in(roberta, X), room(X).</t>
+  </si>
+  <si>
+    <t>... :- married_to(roberta, X), person(X).</t>
+  </si>
+  <si>
+    <t>... :- not married_to(roberta, X), person(X).</t>
+  </si>
+  <si>
+    <t>pNounIsAdjectivePrepositionCNounVariable</t>
+  </si>
+  <si>
+    <t>.* [a-z] is(n't | n't | not | ).* [a-z] \\.$</t>
+  </si>
+  <si>
+    <t>Person X is in room Y.</t>
+  </si>
+  <si>
+    <t>Person X is not in room Y.</t>
+  </si>
+  <si>
+    <t>Person X is married to person Y.</t>
+  </si>
+  <si>
+    <t>Person X is not married to person Y.</t>
+  </si>
+  <si>
+    <t>cNounVariableIsAdjectivePrepositioncNounVariableIs</t>
   </si>
 </sst>
 </file>
@@ -914,8 +1025,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="59">
+  <cellStyleXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -985,7 +1108,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="59">
+  <cellStyles count="71">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1015,6 +1138,12 @@
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1044,6 +1173,12 @@
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1319,17 +1454,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H49"/>
+  <dimension ref="A3:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A9" zoomScale="168" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="C14" zoomScale="168" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.83203125" bestFit="1" customWidth="1"/>
@@ -1650,7 +1785,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>189</v>
+        <v>203</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>12</v>
@@ -1673,7 +1808,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>12</v>
@@ -1696,7 +1831,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>191</v>
+        <v>205</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>12</v>
@@ -1719,7 +1854,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>192</v>
+        <v>206</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>12</v>
@@ -1742,571 +1877,751 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="D20" t="s">
+        <v>193</v>
+      </c>
       <c r="E20" t="s">
-        <v>197</v>
+        <v>189</v>
+      </c>
+      <c r="G20" t="s">
+        <v>200</v>
+      </c>
+      <c r="H20" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="D21" t="s">
+        <v>193</v>
+      </c>
       <c r="E21" t="s">
-        <v>198</v>
+        <v>190</v>
+      </c>
+      <c r="G21" t="s">
+        <v>201</v>
+      </c>
+      <c r="H21" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>195</v>
+        <v>209</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="D22" t="s">
+        <v>193</v>
+      </c>
       <c r="E22" t="s">
-        <v>199</v>
+        <v>191</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="H22" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>196</v>
+        <v>210</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="D23" t="s">
+        <v>193</v>
+      </c>
       <c r="E23" t="s">
-        <v>200</v>
+        <v>192</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>13</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>136</v>
+      <c r="B24" t="s">
+        <v>214</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>140</v>
+        <v>218</v>
       </c>
       <c r="D24" t="s">
-        <v>135</v>
+        <v>231</v>
       </c>
       <c r="E24" t="s">
-        <v>138</v>
-      </c>
-      <c r="G24" t="s">
-        <v>143</v>
-      </c>
-      <c r="H24" t="s">
-        <v>142</v>
+        <v>221</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>14</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>137</v>
+      <c r="B25" t="s">
+        <v>215</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>140</v>
+        <v>218</v>
       </c>
       <c r="D25" t="s">
-        <v>135</v>
+        <v>231</v>
       </c>
       <c r="E25" t="s">
-        <v>139</v>
-      </c>
-      <c r="G25" t="s">
-        <v>144</v>
-      </c>
-      <c r="H25" t="s">
-        <v>141</v>
+        <v>222</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>15</v>
-      </c>
       <c r="B26" t="s">
-        <v>71</v>
+        <v>216</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>68</v>
+        <v>218</v>
       </c>
       <c r="D26" t="s">
-        <v>73</v>
+        <v>231</v>
       </c>
       <c r="E26" t="s">
-        <v>67</v>
-      </c>
-      <c r="G26" t="s">
-        <v>69</v>
-      </c>
-      <c r="H26" t="s">
-        <v>70</v>
+        <v>219</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>16</v>
-      </c>
       <c r="B27" t="s">
-        <v>72</v>
+        <v>217</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>68</v>
+        <v>218</v>
       </c>
       <c r="D27" t="s">
-        <v>73</v>
+        <v>231</v>
       </c>
       <c r="E27" t="s">
-        <v>74</v>
-      </c>
-      <c r="G27" t="s">
-        <v>78</v>
-      </c>
-      <c r="H27" t="s">
-        <v>75</v>
+        <v>220</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>17</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>119</v>
+      <c r="B28" t="s">
+        <v>202</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>77</v>
+        <v>232</v>
       </c>
       <c r="D28" t="s">
-        <v>76</v>
+        <v>237</v>
       </c>
       <c r="E28" t="s">
-        <v>86</v>
-      </c>
-      <c r="G28" t="s">
-        <v>79</v>
-      </c>
-      <c r="H28" t="s">
-        <v>81</v>
-      </c>
+        <v>233</v>
+      </c>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>18</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>83</v>
+      <c r="B29" t="s">
+        <v>211</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>77</v>
+        <v>232</v>
       </c>
       <c r="D29" t="s">
-        <v>76</v>
+        <v>237</v>
       </c>
       <c r="E29" t="s">
-        <v>85</v>
-      </c>
-      <c r="G29" t="s">
-        <v>80</v>
-      </c>
-      <c r="H29" t="s">
-        <v>82</v>
-      </c>
+        <v>234</v>
+      </c>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>19</v>
-      </c>
       <c r="B30" t="s">
-        <v>118</v>
+        <v>212</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>77</v>
+        <v>232</v>
       </c>
       <c r="D30" t="s">
-        <v>76</v>
+        <v>237</v>
       </c>
       <c r="E30" t="s">
-        <v>120</v>
-      </c>
-      <c r="G30" t="s">
-        <v>125</v>
-      </c>
-      <c r="H30" t="s">
-        <v>122</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>20</v>
-      </c>
       <c r="B31" t="s">
-        <v>117</v>
+        <v>213</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>77</v>
+        <v>232</v>
       </c>
       <c r="D31" t="s">
-        <v>76</v>
+        <v>237</v>
       </c>
       <c r="E31" t="s">
-        <v>121</v>
-      </c>
-      <c r="G31" t="s">
-        <v>124</v>
-      </c>
-      <c r="H31" t="s">
-        <v>123</v>
-      </c>
+        <v>236</v>
+      </c>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>90</v>
+        <v>136</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>91</v>
+        <v>140</v>
       </c>
       <c r="D32" t="s">
-        <v>89</v>
+        <v>135</v>
       </c>
       <c r="E32" t="s">
-        <v>87</v>
+        <v>138</v>
       </c>
       <c r="G32" t="s">
-        <v>84</v>
+        <v>143</v>
       </c>
       <c r="H32" t="s">
-        <v>88</v>
+        <v>142</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>95</v>
+        <v>137</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>91</v>
+        <v>140</v>
       </c>
       <c r="D33" t="s">
-        <v>89</v>
+        <v>135</v>
       </c>
       <c r="E33" t="s">
-        <v>92</v>
+        <v>139</v>
       </c>
       <c r="G33" t="s">
-        <v>93</v>
+        <v>144</v>
       </c>
       <c r="H33" t="s">
-        <v>94</v>
+        <v>141</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>23</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>127</v>
+        <v>15</v>
+      </c>
+      <c r="B34" t="s">
+        <v>71</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="D34" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="E34" t="s">
-        <v>129</v>
+        <v>67</v>
       </c>
       <c r="G34" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="H34" t="s">
-        <v>131</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>24</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>128</v>
+        <v>16</v>
+      </c>
+      <c r="B35" t="s">
+        <v>72</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="D35" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="E35" t="s">
-        <v>130</v>
+        <v>74</v>
       </c>
       <c r="G35" t="s">
-        <v>134</v>
+        <v>78</v>
       </c>
       <c r="H35" t="s">
-        <v>132</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>25</v>
-      </c>
-      <c r="B36" t="s">
-        <v>96</v>
+        <v>17</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="D36" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="E36" t="s">
-        <v>100</v>
-      </c>
-      <c r="F36" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="G36" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="H36" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>26</v>
-      </c>
-      <c r="B37" t="s">
-        <v>97</v>
+        <v>18</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="D37" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="E37" t="s">
-        <v>101</v>
-      </c>
-      <c r="F37" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="G37" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="H37" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>27</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>115</v>
+        <v>19</v>
+      </c>
+      <c r="B38" t="s">
+        <v>118</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="D38" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="E38" t="s">
-        <v>108</v>
-      </c>
-      <c r="F38" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="G38" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="H38" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>28</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>116</v>
+        <v>20</v>
+      </c>
+      <c r="B39" t="s">
+        <v>117</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="D39" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="E39" t="s">
-        <v>114</v>
-      </c>
-      <c r="F39" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="G39" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="H39" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>29</v>
-      </c>
-      <c r="B40" t="s">
-        <v>147</v>
+        <v>21</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>145</v>
+        <v>91</v>
       </c>
       <c r="D40" t="s">
-        <v>146</v>
+        <v>89</v>
       </c>
       <c r="E40" t="s">
-        <v>149</v>
+        <v>87</v>
       </c>
       <c r="G40" t="s">
-        <v>153</v>
+        <v>84</v>
       </c>
       <c r="H40" t="s">
-        <v>36</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>148</v>
+        <v>95</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>145</v>
+        <v>91</v>
       </c>
       <c r="D41" t="s">
-        <v>146</v>
+        <v>89</v>
       </c>
       <c r="E41" t="s">
-        <v>150</v>
+        <v>92</v>
       </c>
       <c r="G41" t="s">
-        <v>152</v>
+        <v>93</v>
       </c>
       <c r="H41" t="s">
-        <v>151</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>157</v>
+        <v>127</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>156</v>
+        <v>91</v>
       </c>
       <c r="D42" t="s">
-        <v>155</v>
+        <v>89</v>
       </c>
       <c r="E42" t="s">
-        <v>159</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>154</v>
+        <v>129</v>
+      </c>
+      <c r="G42" t="s">
+        <v>133</v>
+      </c>
+      <c r="H42" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>158</v>
+        <v>128</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>156</v>
+        <v>91</v>
       </c>
       <c r="D43" t="s">
-        <v>155</v>
+        <v>89</v>
       </c>
       <c r="E43" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
       <c r="G43" t="s">
-        <v>160</v>
+        <v>134</v>
+      </c>
+      <c r="H43" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>33</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>164</v>
+        <v>25</v>
+      </c>
+      <c r="B44" t="s">
+        <v>96</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>162</v>
+        <v>98</v>
       </c>
       <c r="D44" t="s">
-        <v>163</v>
+        <v>99</v>
       </c>
       <c r="E44" t="s">
-        <v>167</v>
+        <v>100</v>
+      </c>
+      <c r="F44" t="s">
+        <v>102</v>
       </c>
       <c r="G44" t="s">
-        <v>170</v>
+        <v>103</v>
       </c>
       <c r="H44" t="s">
-        <v>166</v>
+        <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45">
+        <v>26</v>
+      </c>
+      <c r="B45" t="s">
+        <v>97</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D45" t="s">
+        <v>99</v>
+      </c>
+      <c r="E45" t="s">
+        <v>101</v>
+      </c>
+      <c r="F45" t="s">
+        <v>105</v>
+      </c>
+      <c r="G45" t="s">
+        <v>106</v>
+      </c>
+      <c r="H45" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>27</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D46" t="s">
+        <v>99</v>
+      </c>
+      <c r="E46" t="s">
+        <v>108</v>
+      </c>
+      <c r="F46" t="s">
+        <v>109</v>
+      </c>
+      <c r="G46" t="s">
+        <v>110</v>
+      </c>
+      <c r="H46" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>28</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D47" t="s">
+        <v>99</v>
+      </c>
+      <c r="E47" t="s">
+        <v>114</v>
+      </c>
+      <c r="F47" t="s">
+        <v>112</v>
+      </c>
+      <c r="G47" t="s">
+        <v>113</v>
+      </c>
+      <c r="H47" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>29</v>
+      </c>
+      <c r="B48" t="s">
+        <v>147</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D48" t="s">
+        <v>146</v>
+      </c>
+      <c r="E48" t="s">
+        <v>149</v>
+      </c>
+      <c r="G48" t="s">
+        <v>153</v>
+      </c>
+      <c r="H48" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>30</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D49" t="s">
+        <v>146</v>
+      </c>
+      <c r="E49" t="s">
+        <v>150</v>
+      </c>
+      <c r="G49" t="s">
+        <v>152</v>
+      </c>
+      <c r="H49" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>31</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D50" t="s">
+        <v>155</v>
+      </c>
+      <c r="E50" t="s">
+        <v>159</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>32</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D51" t="s">
+        <v>155</v>
+      </c>
+      <c r="E51" t="s">
+        <v>161</v>
+      </c>
+      <c r="G51" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>33</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D52" t="s">
+        <v>163</v>
+      </c>
+      <c r="E52" t="s">
+        <v>167</v>
+      </c>
+      <c r="G52" t="s">
+        <v>170</v>
+      </c>
+      <c r="H52" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53">
         <v>34</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B53" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C53" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D53" t="s">
         <v>163</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E53" t="s">
         <v>168</v>
       </c>
-      <c r="G45" t="s">
+      <c r="G53" t="s">
         <v>169</v>
       </c>
-      <c r="H45" s="5" t="s">
+      <c r="H53" s="5" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B46" s="2"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B47" s="2"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B48" s="2"/>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B49" s="2"/>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B54" s="2"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B55" s="2"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B56" s="2"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B57" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
gui: added save function
</commit_message>
<xml_diff>
--- a/sentences.xlsx
+++ b/sentences.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="250">
   <si>
     <t>Structure</t>
   </si>
@@ -941,6 +941,42 @@
   </si>
   <si>
     <t>cNounVariableIsAdjectivePrepositioncNounVariableIs</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - in(X, Y) :- ...</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - married_to(X, Y) :- ...</t>
+  </si>
+  <si>
+    <t>... :- in(X, Y), person(X), room(Y).</t>
+  </si>
+  <si>
+    <t>married_to(X, Y) :- ...</t>
+  </si>
+  <si>
+    <t>in(X, Y) :- ...</t>
+  </si>
+  <si>
+    <t>... :- not in(X, Y), person(X), room(Y).</t>
+  </si>
+  <si>
+    <t>... :- married_to(X, Y), person(X), person(Y).</t>
+  </si>
+  <si>
+    <t>... :- not married_to(X, Y), person(X), person(Y).</t>
+  </si>
+  <si>
+    <t>PNoun is Verb.</t>
+  </si>
+  <si>
+    <t>CNoun Variable is Verb.</t>
+  </si>
+  <si>
+    <t>.* is(n't | n't | not | ).* \\.$</t>
+  </si>
+  <si>
+    <t>.* [a-z] is(n't | n't | not | ).* \\.$</t>
   </si>
 </sst>
 </file>
@@ -1025,8 +1061,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="71">
+  <cellStyleXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1108,7 +1146,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="71">
+  <cellStyles count="73">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1144,6 +1182,7 @@
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1179,6 +1218,7 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1454,21 +1494,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H57"/>
+  <dimension ref="A3:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="C14" zoomScale="168" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A4" zoomScale="168" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1640,63 +1680,27 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
+      <c r="B10" s="2" t="s">
+        <v>246</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" t="s">
-        <v>57</v>
-      </c>
-      <c r="H10" t="s">
-        <v>55</v>
+        <v>248</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>16</v>
+      <c r="B11" s="2" t="s">
+        <v>247</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" t="s">
-        <v>58</v>
-      </c>
-      <c r="H11" t="s">
-        <v>56</v>
+        <v>249</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>9</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>59</v>
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>12</v>
@@ -1705,21 +1709,24 @@
         <v>13</v>
       </c>
       <c r="E12" t="s">
-        <v>61</v>
+        <v>14</v>
+      </c>
+      <c r="F12" t="s">
+        <v>15</v>
       </c>
       <c r="G12" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H12" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>10</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>60</v>
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>12</v>
@@ -1728,110 +1735,116 @@
         <v>13</v>
       </c>
       <c r="E13" t="s">
-        <v>62</v>
+        <v>18</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
       </c>
       <c r="G13" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H13" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>11</v>
-      </c>
-      <c r="B14" t="s">
-        <v>19</v>
+        <v>9</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="G14" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="H14" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
+        <v>10</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B15" t="s">
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" t="s">
+        <v>64</v>
+      </c>
+      <c r="H15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" t="s">
+        <v>47</v>
+      </c>
+      <c r="H16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D17" t="s">
         <v>20</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E17" t="s">
         <v>27</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G17" t="s">
         <v>48</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H17" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
         <v>203</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" t="s">
-        <v>174</v>
-      </c>
-      <c r="E16" t="s">
-        <v>172</v>
-      </c>
-      <c r="F16" t="s">
-        <v>175</v>
-      </c>
-      <c r="G16" t="s">
-        <v>176</v>
-      </c>
-      <c r="H16" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>204</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E17" t="s">
-        <v>173</v>
-      </c>
-      <c r="F17" t="s">
-        <v>178</v>
-      </c>
-      <c r="G17" t="s">
-        <v>177</v>
-      </c>
-      <c r="H17" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>205</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>12</v>
@@ -1840,21 +1853,24 @@
         <v>174</v>
       </c>
       <c r="E18" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="F18" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="G18" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="H18" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>14</v>
+      </c>
       <c r="B19" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>12</v>
@@ -1863,61 +1879,76 @@
         <v>174</v>
       </c>
       <c r="E19" t="s">
+        <v>173</v>
+      </c>
+      <c r="F19" t="s">
+        <v>178</v>
+      </c>
+      <c r="G19" t="s">
+        <v>177</v>
+      </c>
+      <c r="H19" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>205</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" t="s">
+        <v>174</v>
+      </c>
+      <c r="E20" t="s">
+        <v>181</v>
+      </c>
+      <c r="F20" t="s">
+        <v>183</v>
+      </c>
+      <c r="G20" t="s">
+        <v>184</v>
+      </c>
+      <c r="H20" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>16</v>
+      </c>
+      <c r="B21" t="s">
+        <v>206</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>174</v>
+      </c>
+      <c r="E21" t="s">
         <v>182</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F21" t="s">
         <v>186</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G21" t="s">
         <v>185</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H21" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
         <v>207</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" t="s">
-        <v>193</v>
-      </c>
-      <c r="E20" t="s">
-        <v>189</v>
-      </c>
-      <c r="G20" t="s">
-        <v>200</v>
-      </c>
-      <c r="H20" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
-        <v>208</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" t="s">
-        <v>193</v>
-      </c>
-      <c r="E21" t="s">
-        <v>190</v>
-      </c>
-      <c r="G21" t="s">
-        <v>201</v>
-      </c>
-      <c r="H21" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>209</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>28</v>
@@ -1926,18 +1957,21 @@
         <v>193</v>
       </c>
       <c r="E22" t="s">
-        <v>191</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>196</v>
+        <v>189</v>
+      </c>
+      <c r="G22" t="s">
+        <v>200</v>
       </c>
       <c r="H22" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>18</v>
+      </c>
       <c r="B23" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>28</v>
@@ -1946,58 +1980,67 @@
         <v>193</v>
       </c>
       <c r="E23" t="s">
+        <v>190</v>
+      </c>
+      <c r="G23" t="s">
+        <v>201</v>
+      </c>
+      <c r="H23" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>19</v>
+      </c>
+      <c r="B24" t="s">
+        <v>209</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" t="s">
+        <v>193</v>
+      </c>
+      <c r="E24" t="s">
+        <v>191</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="H24" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>20</v>
+      </c>
+      <c r="B25" t="s">
+        <v>210</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" t="s">
+        <v>193</v>
+      </c>
+      <c r="E25" t="s">
         <v>192</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="G25" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="H25" s="5" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>21</v>
+      </c>
+      <c r="B26" t="s">
         <v>214</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="D24" t="s">
-        <v>231</v>
-      </c>
-      <c r="E24" t="s">
-        <v>221</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
-        <v>215</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="D25" t="s">
-        <v>231</v>
-      </c>
-      <c r="E25" t="s">
-        <v>222</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
-        <v>216</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>218</v>
@@ -2006,18 +2049,21 @@
         <v>231</v>
       </c>
       <c r="E26" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>22</v>
+      </c>
       <c r="B27" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>218</v>
@@ -2026,50 +2072,67 @@
         <v>231</v>
       </c>
       <c r="E27" t="s">
+        <v>222</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>23</v>
+      </c>
+      <c r="B28" t="s">
+        <v>216</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D28" t="s">
+        <v>231</v>
+      </c>
+      <c r="E28" t="s">
+        <v>219</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>24</v>
+      </c>
+      <c r="B29" t="s">
+        <v>217</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D29" t="s">
+        <v>231</v>
+      </c>
+      <c r="E29" t="s">
         <v>220</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="G29" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="H29" s="5" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>25</v>
+      </c>
+      <c r="B30" t="s">
         <v>202</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="D28" t="s">
-        <v>237</v>
-      </c>
-      <c r="E28" t="s">
-        <v>233</v>
-      </c>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
-        <v>211</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="D29" t="s">
-        <v>237</v>
-      </c>
-      <c r="E29" t="s">
-        <v>234</v>
-      </c>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
-        <v>212</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>232</v>
@@ -2078,14 +2141,21 @@
         <v>237</v>
       </c>
       <c r="E30" t="s">
-        <v>235</v>
-      </c>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
+        <v>233</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>26</v>
+      </c>
       <c r="B31" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>232</v>
@@ -2094,155 +2164,159 @@
         <v>237</v>
       </c>
       <c r="E31" t="s">
-        <v>236</v>
-      </c>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
+        <v>234</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>13</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>136</v>
+        <v>27</v>
+      </c>
+      <c r="B32" t="s">
+        <v>212</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>140</v>
+        <v>232</v>
       </c>
       <c r="D32" t="s">
-        <v>135</v>
+        <v>237</v>
       </c>
       <c r="E32" t="s">
-        <v>138</v>
-      </c>
-      <c r="G32" t="s">
-        <v>143</v>
-      </c>
-      <c r="H32" t="s">
-        <v>142</v>
+        <v>235</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>14</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>137</v>
+        <v>28</v>
+      </c>
+      <c r="B33" t="s">
+        <v>213</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>140</v>
+        <v>232</v>
       </c>
       <c r="D33" t="s">
-        <v>135</v>
+        <v>237</v>
       </c>
       <c r="E33" t="s">
-        <v>139</v>
-      </c>
-      <c r="G33" t="s">
-        <v>144</v>
-      </c>
-      <c r="H33" t="s">
-        <v>141</v>
+        <v>236</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>15</v>
-      </c>
-      <c r="B34" t="s">
-        <v>71</v>
+        <v>29</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>68</v>
+        <v>140</v>
       </c>
       <c r="D34" t="s">
-        <v>73</v>
+        <v>135</v>
       </c>
       <c r="E34" t="s">
-        <v>67</v>
+        <v>138</v>
       </c>
       <c r="G34" t="s">
-        <v>69</v>
+        <v>143</v>
       </c>
       <c r="H34" t="s">
-        <v>70</v>
+        <v>142</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>16</v>
-      </c>
-      <c r="B35" t="s">
-        <v>72</v>
+        <v>30</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>137</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>68</v>
+        <v>140</v>
       </c>
       <c r="D35" t="s">
-        <v>73</v>
+        <v>135</v>
       </c>
       <c r="E35" t="s">
-        <v>74</v>
+        <v>139</v>
       </c>
       <c r="G35" t="s">
-        <v>78</v>
+        <v>144</v>
       </c>
       <c r="H35" t="s">
-        <v>75</v>
+        <v>141</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>17</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>119</v>
+        <v>31</v>
+      </c>
+      <c r="B36" t="s">
+        <v>71</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D36" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E36" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="G36" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="H36" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>18</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>83</v>
+        <v>32</v>
+      </c>
+      <c r="B37" t="s">
+        <v>72</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D37" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E37" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="G37" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H37" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>19</v>
-      </c>
-      <c r="B38" t="s">
-        <v>118</v>
+        <v>33</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>77</v>
@@ -2251,21 +2325,21 @@
         <v>76</v>
       </c>
       <c r="E38" t="s">
-        <v>120</v>
+        <v>86</v>
       </c>
       <c r="G38" t="s">
-        <v>125</v>
+        <v>79</v>
       </c>
       <c r="H38" t="s">
-        <v>122</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>20</v>
-      </c>
-      <c r="B39" t="s">
-        <v>117</v>
+        <v>34</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>77</v>
@@ -2274,67 +2348,67 @@
         <v>76</v>
       </c>
       <c r="E39" t="s">
-        <v>121</v>
+        <v>85</v>
       </c>
       <c r="G39" t="s">
-        <v>124</v>
+        <v>80</v>
       </c>
       <c r="H39" t="s">
-        <v>123</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>21</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>90</v>
+        <v>35</v>
+      </c>
+      <c r="B40" t="s">
+        <v>118</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D40" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E40" t="s">
-        <v>87</v>
+        <v>120</v>
       </c>
       <c r="G40" t="s">
-        <v>84</v>
+        <v>125</v>
       </c>
       <c r="H40" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>22</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>95</v>
+        <v>36</v>
+      </c>
+      <c r="B41" t="s">
+        <v>117</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D41" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E41" t="s">
-        <v>92</v>
+        <v>121</v>
       </c>
       <c r="G41" t="s">
-        <v>93</v>
+        <v>124</v>
       </c>
       <c r="H41" t="s">
-        <v>94</v>
+        <v>123</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>127</v>
+        <v>90</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>91</v>
@@ -2343,21 +2417,21 @@
         <v>89</v>
       </c>
       <c r="E42" t="s">
-        <v>129</v>
+        <v>87</v>
       </c>
       <c r="G42" t="s">
-        <v>133</v>
+        <v>84</v>
       </c>
       <c r="H42" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>128</v>
+        <v>95</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>91</v>
@@ -2366,73 +2440,67 @@
         <v>89</v>
       </c>
       <c r="E43" t="s">
-        <v>130</v>
+        <v>92</v>
       </c>
       <c r="G43" t="s">
-        <v>134</v>
+        <v>93</v>
       </c>
       <c r="H43" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>25</v>
-      </c>
-      <c r="B44" t="s">
-        <v>96</v>
+        <v>39</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D44" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="E44" t="s">
-        <v>100</v>
-      </c>
-      <c r="F44" t="s">
-        <v>102</v>
+        <v>129</v>
       </c>
       <c r="G44" t="s">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="H44" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>26</v>
-      </c>
-      <c r="B45" t="s">
-        <v>97</v>
+        <v>40</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D45" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="E45" t="s">
-        <v>101</v>
-      </c>
-      <c r="F45" t="s">
-        <v>105</v>
+        <v>130</v>
       </c>
       <c r="G45" t="s">
-        <v>106</v>
+        <v>134</v>
       </c>
       <c r="H45" t="s">
-        <v>107</v>
+        <v>132</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>27</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>115</v>
+        <v>41</v>
+      </c>
+      <c r="B46" t="s">
+        <v>96</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>98</v>
@@ -2441,24 +2509,24 @@
         <v>99</v>
       </c>
       <c r="E46" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="F46" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="G46" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="H46" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>28</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>116</v>
+        <v>42</v>
+      </c>
+      <c r="B47" t="s">
+        <v>97</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>98</v>
@@ -2467,161 +2535,213 @@
         <v>99</v>
       </c>
       <c r="E47" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="F47" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="G47" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="H47" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>29</v>
-      </c>
-      <c r="B48" t="s">
-        <v>147</v>
+        <v>43</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>145</v>
+        <v>98</v>
       </c>
       <c r="D48" t="s">
-        <v>146</v>
+        <v>99</v>
       </c>
       <c r="E48" t="s">
-        <v>149</v>
+        <v>108</v>
+      </c>
+      <c r="F48" t="s">
+        <v>109</v>
       </c>
       <c r="G48" t="s">
-        <v>153</v>
+        <v>110</v>
       </c>
       <c r="H48" t="s">
-        <v>36</v>
+        <v>111</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>148</v>
+        <v>116</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>145</v>
+        <v>98</v>
       </c>
       <c r="D49" t="s">
-        <v>146</v>
+        <v>99</v>
       </c>
       <c r="E49" t="s">
-        <v>150</v>
+        <v>114</v>
+      </c>
+      <c r="F49" t="s">
+        <v>112</v>
       </c>
       <c r="G49" t="s">
-        <v>152</v>
+        <v>113</v>
       </c>
       <c r="H49" t="s">
-        <v>151</v>
+        <v>126</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>31</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>157</v>
+        <v>45</v>
+      </c>
+      <c r="B50" t="s">
+        <v>147</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="D50" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="E50" t="s">
-        <v>159</v>
-      </c>
-      <c r="G50" s="5" t="s">
-        <v>154</v>
+        <v>149</v>
+      </c>
+      <c r="G50" t="s">
+        <v>153</v>
+      </c>
+      <c r="H50" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="D51" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="E51" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="G51" t="s">
-        <v>160</v>
+        <v>152</v>
+      </c>
+      <c r="H51" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D52" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="E52" t="s">
-        <v>167</v>
-      </c>
-      <c r="G52" t="s">
-        <v>170</v>
-      </c>
-      <c r="H52" t="s">
-        <v>166</v>
+        <v>159</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="B53" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D53" t="s">
+        <v>155</v>
+      </c>
+      <c r="E53" t="s">
+        <v>161</v>
+      </c>
+      <c r="G53" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>49</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D54" t="s">
+        <v>163</v>
+      </c>
+      <c r="E54" t="s">
+        <v>167</v>
+      </c>
+      <c r="G54" t="s">
+        <v>170</v>
+      </c>
+      <c r="H54" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>50</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C55" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D55" t="s">
         <v>163</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E55" t="s">
         <v>168</v>
       </c>
-      <c r="G53" t="s">
+      <c r="G55" t="s">
         <v>169</v>
       </c>
-      <c r="H53" s="5" t="s">
+      <c r="H55" s="5" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B54" s="2"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B55" s="2"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B56" s="2"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B57" s="2"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B58" s="2"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B59" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added "PNoun Verb.", "CNoun Variable Verb.", "PNoun is Verb.", "CNoun Variable is Verb."
</commit_message>
<xml_diff>
--- a/sentences.xlsx
+++ b/sentences.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="279">
   <si>
     <t>Structure</t>
   </si>
@@ -973,10 +973,97 @@
     <t>CNoun Variable is Verb.</t>
   </si>
   <si>
-    <t>.* is(n't | n't | not | ).* \\.$</t>
-  </si>
-  <si>
-    <t>.* [a-z] is(n't | n't | not | ).* \\.$</t>
+    <t>PNoun Verb.</t>
+  </si>
+  <si>
+    <t>CNoun Variable Verb.</t>
+  </si>
+  <si>
+    <t>pNounVerb</t>
+  </si>
+  <si>
+    <t>cNounVariableVerb</t>
+  </si>
+  <si>
+    <t>pNounIsVerb</t>
+  </si>
+  <si>
+    <t>cNounVariableisVerb</t>
+  </si>
+  <si>
+    <t>Roberta reads.</t>
+  </si>
+  <si>
+    <t>Person X reads.</t>
+  </si>
+  <si>
+    <t>Roberta is reading.</t>
+  </si>
+  <si>
+    <t>Person X is reading.</t>
+  </si>
+  <si>
+    <t>read(roberta).</t>
+  </si>
+  <si>
+    <t>read(roberta) :- ...</t>
+  </si>
+  <si>
+    <t>Pnoun not Verb.</t>
+  </si>
+  <si>
+    <t>Roberta does not read.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - read(roberta).</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - read(roberta) :- ...</t>
+  </si>
+  <si>
+    <t>... :- read(roberta).</t>
+  </si>
+  <si>
+    <t>... :- not read(roberta).</t>
+  </si>
+  <si>
+    <t>read(X) :- ...</t>
+  </si>
+  <si>
+    <t>... :- read(X), person(X).</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - read(X) :- ...</t>
+  </si>
+  <si>
+    <t>... :- not read(X), person(X).</t>
+  </si>
+  <si>
+    <t>Person X does not read.</t>
+  </si>
+  <si>
+    <t>Roberta is not reading.</t>
+  </si>
+  <si>
+    <t>CNoun Variable not Verb.</t>
+  </si>
+  <si>
+    <t>PNoun is not Verb.</t>
+  </si>
+  <si>
+    <t>CNoun Variable is not Verb.</t>
+  </si>
+  <si>
+    <t>.* is(n't | n't | not | ).*\\.$</t>
+  </si>
+  <si>
+    <t>.* [a-z] .*\\.$</t>
+  </si>
+  <si>
+    <t>.* .*\\.$</t>
+  </si>
+  <si>
+    <t>Person X is not reading.</t>
   </si>
 </sst>
 </file>
@@ -1061,7 +1148,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="73">
+  <cellStyleXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1135,8 +1222,34 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1145,8 +1258,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="73">
+  <cellStyles count="99">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1183,6 +1302,19 @@
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1219,6 +1351,19 @@
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1494,10 +1639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H59"/>
+  <dimension ref="A3:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A4" zoomScale="168" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" zoomScale="108" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1679,1069 +1824,1249 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="2" t="s">
+    <row r="10" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
+        <v>7</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
+        <v>8</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
+        <v>9</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
+        <v>10</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
+        <v>11</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="2" t="s">
+      <c r="C14" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="6">
+        <v>12</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="6">
+        <v>13</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>7</v>
-      </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="C16" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="6">
         <v>14</v>
       </c>
-      <c r="F12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" t="s">
-        <v>57</v>
-      </c>
-      <c r="H12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>8</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13" t="s">
-        <v>58</v>
-      </c>
-      <c r="H13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>9</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" t="s">
-        <v>61</v>
-      </c>
-      <c r="G14" t="s">
-        <v>63</v>
-      </c>
-      <c r="H14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>10</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" t="s">
-        <v>62</v>
-      </c>
-      <c r="G15" t="s">
-        <v>64</v>
-      </c>
-      <c r="H15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>11</v>
-      </c>
-      <c r="B16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="1" t="s">
+      <c r="B17" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" t="s">
-        <v>21</v>
-      </c>
-      <c r="G16" t="s">
-        <v>47</v>
-      </c>
-      <c r="H16" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>12</v>
-      </c>
-      <c r="B17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" t="s">
-        <v>27</v>
-      </c>
-      <c r="G17" t="s">
-        <v>48</v>
-      </c>
-      <c r="H17" t="s">
-        <v>50</v>
+      <c r="D17" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>203</v>
+        <v>11</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>174</v>
+        <v>13</v>
       </c>
       <c r="E18" t="s">
-        <v>172</v>
+        <v>14</v>
       </c>
       <c r="F18" t="s">
-        <v>175</v>
+        <v>15</v>
       </c>
       <c r="G18" t="s">
-        <v>176</v>
+        <v>57</v>
       </c>
       <c r="H18" t="s">
-        <v>180</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>204</v>
+        <v>16</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>174</v>
+        <v>13</v>
       </c>
       <c r="E19" t="s">
-        <v>173</v>
+        <v>18</v>
       </c>
       <c r="F19" t="s">
-        <v>178</v>
+        <v>17</v>
       </c>
       <c r="G19" t="s">
-        <v>177</v>
+        <v>58</v>
       </c>
       <c r="H19" t="s">
-        <v>179</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>15</v>
-      </c>
-      <c r="B20" t="s">
-        <v>205</v>
+        <v>17</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>174</v>
+        <v>13</v>
       </c>
       <c r="E20" t="s">
-        <v>181</v>
-      </c>
-      <c r="F20" t="s">
-        <v>183</v>
+        <v>61</v>
       </c>
       <c r="G20" t="s">
-        <v>184</v>
+        <v>63</v>
       </c>
       <c r="H20" t="s">
-        <v>187</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>16</v>
-      </c>
-      <c r="B21" t="s">
-        <v>206</v>
+        <v>18</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D21" t="s">
-        <v>174</v>
+        <v>13</v>
       </c>
       <c r="E21" t="s">
-        <v>182</v>
-      </c>
-      <c r="F21" t="s">
-        <v>186</v>
+        <v>62</v>
       </c>
       <c r="G21" t="s">
-        <v>185</v>
+        <v>64</v>
       </c>
       <c r="H21" t="s">
-        <v>188</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>207</v>
+        <v>19</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D22" t="s">
-        <v>193</v>
+        <v>20</v>
       </c>
       <c r="E22" t="s">
-        <v>189</v>
+        <v>21</v>
       </c>
       <c r="G22" t="s">
-        <v>200</v>
+        <v>47</v>
       </c>
       <c r="H22" t="s">
-        <v>198</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>208</v>
+        <v>26</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D23" t="s">
-        <v>193</v>
+        <v>20</v>
       </c>
       <c r="E23" t="s">
-        <v>190</v>
+        <v>27</v>
       </c>
       <c r="G23" t="s">
-        <v>201</v>
+        <v>48</v>
       </c>
       <c r="H23" t="s">
-        <v>199</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="E24" t="s">
-        <v>191</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>196</v>
+        <v>172</v>
+      </c>
+      <c r="F24" t="s">
+        <v>175</v>
+      </c>
+      <c r="G24" t="s">
+        <v>176</v>
       </c>
       <c r="H24" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="D25" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="E25" t="s">
-        <v>192</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>195</v>
+        <v>173</v>
+      </c>
+      <c r="F25" t="s">
+        <v>178</v>
+      </c>
+      <c r="G25" t="s">
+        <v>177</v>
+      </c>
+      <c r="H25" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>218</v>
+        <v>12</v>
       </c>
       <c r="D26" t="s">
-        <v>231</v>
+        <v>174</v>
       </c>
       <c r="E26" t="s">
-        <v>221</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="H26" s="5" t="s">
-        <v>223</v>
+        <v>181</v>
+      </c>
+      <c r="F26" t="s">
+        <v>183</v>
+      </c>
+      <c r="G26" t="s">
+        <v>184</v>
+      </c>
+      <c r="H26" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>218</v>
+        <v>12</v>
       </c>
       <c r="D27" t="s">
-        <v>231</v>
+        <v>174</v>
       </c>
       <c r="E27" t="s">
-        <v>222</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>224</v>
+        <v>182</v>
+      </c>
+      <c r="F27" t="s">
+        <v>186</v>
+      </c>
+      <c r="G27" t="s">
+        <v>185</v>
+      </c>
+      <c r="H27" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>218</v>
+        <v>28</v>
       </c>
       <c r="D28" t="s">
-        <v>231</v>
+        <v>193</v>
       </c>
       <c r="E28" t="s">
-        <v>219</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>225</v>
+        <v>189</v>
+      </c>
+      <c r="G28" t="s">
+        <v>200</v>
+      </c>
+      <c r="H28" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>218</v>
+        <v>28</v>
       </c>
       <c r="D29" t="s">
-        <v>231</v>
+        <v>193</v>
       </c>
       <c r="E29" t="s">
-        <v>220</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>226</v>
+        <v>190</v>
+      </c>
+      <c r="G29" t="s">
+        <v>201</v>
+      </c>
+      <c r="H29" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>232</v>
+        <v>28</v>
       </c>
       <c r="D30" t="s">
-        <v>237</v>
+        <v>193</v>
       </c>
       <c r="E30" t="s">
-        <v>233</v>
+        <v>191</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>242</v>
+        <v>196</v>
+      </c>
+      <c r="H30" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>232</v>
+        <v>28</v>
       </c>
       <c r="D31" t="s">
-        <v>237</v>
+        <v>193</v>
       </c>
       <c r="E31" t="s">
-        <v>234</v>
+        <v>192</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>243</v>
+        <v>197</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>238</v>
+        <v>195</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="D32" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="E32" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>244</v>
+        <v>227</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="D33" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="E33" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>29</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>136</v>
+        <v>31</v>
+      </c>
+      <c r="B34" t="s">
+        <v>216</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>140</v>
+        <v>218</v>
       </c>
       <c r="D34" t="s">
-        <v>135</v>
+        <v>231</v>
       </c>
       <c r="E34" t="s">
-        <v>138</v>
-      </c>
-      <c r="G34" t="s">
-        <v>143</v>
-      </c>
-      <c r="H34" t="s">
-        <v>142</v>
+        <v>219</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>30</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>137</v>
+        <v>32</v>
+      </c>
+      <c r="B35" t="s">
+        <v>217</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>140</v>
+        <v>218</v>
       </c>
       <c r="D35" t="s">
-        <v>135</v>
+        <v>231</v>
       </c>
       <c r="E35" t="s">
-        <v>139</v>
-      </c>
-      <c r="G35" t="s">
-        <v>144</v>
-      </c>
-      <c r="H35" t="s">
-        <v>141</v>
+        <v>220</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>71</v>
+        <v>202</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>68</v>
+        <v>232</v>
       </c>
       <c r="D36" t="s">
-        <v>73</v>
+        <v>237</v>
       </c>
       <c r="E36" t="s">
-        <v>67</v>
-      </c>
-      <c r="G36" t="s">
-        <v>69</v>
-      </c>
-      <c r="H36" t="s">
-        <v>70</v>
+        <v>233</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>72</v>
+        <v>211</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>68</v>
+        <v>232</v>
       </c>
       <c r="D37" t="s">
-        <v>73</v>
+        <v>237</v>
       </c>
       <c r="E37" t="s">
-        <v>74</v>
-      </c>
-      <c r="G37" t="s">
-        <v>78</v>
-      </c>
-      <c r="H37" t="s">
-        <v>75</v>
+        <v>234</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>33</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>119</v>
+        <v>35</v>
+      </c>
+      <c r="B38" t="s">
+        <v>212</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>77</v>
+        <v>232</v>
       </c>
       <c r="D38" t="s">
-        <v>76</v>
+        <v>237</v>
       </c>
       <c r="E38" t="s">
-        <v>86</v>
-      </c>
-      <c r="G38" t="s">
-        <v>79</v>
-      </c>
-      <c r="H38" t="s">
-        <v>81</v>
+        <v>235</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>34</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>83</v>
+        <v>36</v>
+      </c>
+      <c r="B39" t="s">
+        <v>213</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>77</v>
+        <v>232</v>
       </c>
       <c r="D39" t="s">
-        <v>76</v>
+        <v>237</v>
       </c>
       <c r="E39" t="s">
-        <v>85</v>
-      </c>
-      <c r="G39" t="s">
-        <v>80</v>
-      </c>
-      <c r="H39" t="s">
-        <v>82</v>
+        <v>236</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>35</v>
-      </c>
-      <c r="B40" t="s">
-        <v>118</v>
+        <v>37</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>77</v>
+        <v>140</v>
       </c>
       <c r="D40" t="s">
-        <v>76</v>
+        <v>135</v>
       </c>
       <c r="E40" t="s">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="G40" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="H40" t="s">
-        <v>122</v>
+        <v>142</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>36</v>
-      </c>
-      <c r="B41" t="s">
-        <v>117</v>
+        <v>38</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>137</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>77</v>
+        <v>140</v>
       </c>
       <c r="D41" t="s">
-        <v>76</v>
+        <v>135</v>
       </c>
       <c r="E41" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="G41" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="H41" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>37</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>90</v>
+        <v>39</v>
+      </c>
+      <c r="B42" t="s">
+        <v>71</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="D42" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="E42" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="G42" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="H42" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>38</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>95</v>
+        <v>40</v>
+      </c>
+      <c r="B43" t="s">
+        <v>72</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="D43" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="E43" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="G43" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="H43" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D44" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E44" t="s">
-        <v>129</v>
+        <v>86</v>
       </c>
       <c r="G44" t="s">
-        <v>133</v>
+        <v>79</v>
       </c>
       <c r="H44" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>128</v>
+        <v>83</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D45" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E45" t="s">
-        <v>130</v>
+        <v>85</v>
       </c>
       <c r="G45" t="s">
-        <v>134</v>
+        <v>80</v>
       </c>
       <c r="H45" t="s">
-        <v>132</v>
+        <v>82</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B46" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="D46" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="E46" t="s">
-        <v>100</v>
-      </c>
-      <c r="F46" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="G46" t="s">
-        <v>103</v>
+        <v>125</v>
       </c>
       <c r="H46" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B47" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="D47" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="E47" t="s">
-        <v>101</v>
-      </c>
-      <c r="F47" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="G47" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="H47" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D48" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="E48" t="s">
-        <v>108</v>
-      </c>
-      <c r="F48" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="G48" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
       <c r="H48" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D49" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="E49" t="s">
-        <v>114</v>
-      </c>
-      <c r="F49" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="G49" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="H49" t="s">
-        <v>126</v>
+        <v>94</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>45</v>
-      </c>
-      <c r="B50" t="s">
-        <v>147</v>
+        <v>47</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>145</v>
+        <v>91</v>
       </c>
       <c r="D50" t="s">
-        <v>146</v>
+        <v>89</v>
       </c>
       <c r="E50" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="G50" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
       <c r="H50" t="s">
-        <v>36</v>
+        <v>131</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>145</v>
+        <v>91</v>
       </c>
       <c r="D51" t="s">
-        <v>146</v>
+        <v>89</v>
       </c>
       <c r="E51" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="G51" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="H51" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>47</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>157</v>
+        <v>49</v>
+      </c>
+      <c r="B52" t="s">
+        <v>96</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>156</v>
+        <v>98</v>
       </c>
       <c r="D52" t="s">
-        <v>155</v>
+        <v>99</v>
       </c>
       <c r="E52" t="s">
-        <v>159</v>
-      </c>
-      <c r="G52" s="5" t="s">
-        <v>154</v>
+        <v>100</v>
+      </c>
+      <c r="F52" t="s">
+        <v>102</v>
+      </c>
+      <c r="G52" t="s">
+        <v>103</v>
+      </c>
+      <c r="H52" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>48</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>158</v>
+        <v>50</v>
+      </c>
+      <c r="B53" t="s">
+        <v>97</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>156</v>
+        <v>98</v>
       </c>
       <c r="D53" t="s">
-        <v>155</v>
+        <v>99</v>
       </c>
       <c r="E53" t="s">
-        <v>161</v>
+        <v>101</v>
+      </c>
+      <c r="F53" t="s">
+        <v>105</v>
       </c>
       <c r="G53" t="s">
-        <v>160</v>
+        <v>106</v>
+      </c>
+      <c r="H53" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>164</v>
+        <v>115</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>162</v>
+        <v>98</v>
       </c>
       <c r="D54" t="s">
-        <v>163</v>
+        <v>99</v>
       </c>
       <c r="E54" t="s">
-        <v>167</v>
+        <v>108</v>
+      </c>
+      <c r="F54" t="s">
+        <v>109</v>
       </c>
       <c r="G54" t="s">
-        <v>170</v>
+        <v>110</v>
       </c>
       <c r="H54" t="s">
-        <v>166</v>
+        <v>111</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B55" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D55" t="s">
+        <v>99</v>
+      </c>
+      <c r="E55" t="s">
+        <v>114</v>
+      </c>
+      <c r="F55" t="s">
+        <v>112</v>
+      </c>
+      <c r="G55" t="s">
+        <v>113</v>
+      </c>
+      <c r="H55" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>53</v>
+      </c>
+      <c r="B56" t="s">
+        <v>147</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D56" t="s">
+        <v>146</v>
+      </c>
+      <c r="E56" t="s">
+        <v>149</v>
+      </c>
+      <c r="G56" t="s">
+        <v>153</v>
+      </c>
+      <c r="H56" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>54</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D57" t="s">
+        <v>146</v>
+      </c>
+      <c r="E57" t="s">
+        <v>150</v>
+      </c>
+      <c r="G57" t="s">
+        <v>152</v>
+      </c>
+      <c r="H57" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>55</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D58" t="s">
+        <v>155</v>
+      </c>
+      <c r="E58" t="s">
+        <v>159</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>56</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D59" t="s">
+        <v>155</v>
+      </c>
+      <c r="E59" t="s">
+        <v>161</v>
+      </c>
+      <c r="G59" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>57</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D60" t="s">
+        <v>163</v>
+      </c>
+      <c r="E60" t="s">
+        <v>167</v>
+      </c>
+      <c r="G60" t="s">
+        <v>170</v>
+      </c>
+      <c r="H60" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>58</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C61" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D61" t="s">
         <v>163</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E61" t="s">
         <v>168</v>
       </c>
-      <c r="G55" t="s">
+      <c r="G61" t="s">
         <v>169</v>
       </c>
-      <c r="H55" s="5" t="s">
+      <c r="H61" s="5" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B56" s="2"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B57" s="2"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B58" s="2"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B59" s="2"/>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B62" s="2"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B63" s="2"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B64" s="2"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B65" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed "PNoun is Adjective PNoun."
</commit_message>
<xml_diff>
--- a/sentences.xlsx
+++ b/sentences.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="297">
   <si>
     <t>Structure</t>
   </si>
@@ -940,9 +940,6 @@
     <t>Person X is not married to person Y.</t>
   </si>
   <si>
-    <t>cNounVariableIsAdjectivePrepositioncNounVariableIs</t>
-  </si>
-  <si>
     <t xml:space="preserve"> - in(X, Y) :- ...</t>
   </si>
   <si>
@@ -1064,6 +1061,83 @@
   </si>
   <si>
     <t>Person X is not reading.</t>
+  </si>
+  <si>
+    <t>cNounVariableVerbPnoun</t>
+  </si>
+  <si>
+    <r>
+      <t>.* [a-z] .*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+      </rPr>
+      <t>\\</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+      </rPr>
+      <t>.$</t>
+    </r>
+  </si>
+  <si>
+    <t>CNoun Variable Verb PNoun.</t>
+  </si>
+  <si>
+    <t>CNoun Variable Verb Preposition PNoun.</t>
+  </si>
+  <si>
+    <t>CNoun Variable not Verb Preposition PNoun.</t>
+  </si>
+  <si>
+    <t>CNoun Variable not Verb PNoun.</t>
+  </si>
+  <si>
+    <t>Person X studies computer science.</t>
+  </si>
+  <si>
+    <t>Person X does not studies computer science.</t>
+  </si>
+  <si>
+    <t>Person X studies at TU Wien.</t>
+  </si>
+  <si>
+    <t>Person X does not study at TU Wien.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - study_at(X, tuwien) :- ...</t>
+  </si>
+  <si>
+    <t>study_at(X, tuwien) :- ...</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - study(X, computerscience) :- ...</t>
+  </si>
+  <si>
+    <t>study(X, computerscience) :- ...</t>
+  </si>
+  <si>
+    <t>... :- study(X, computerscience), person(X).</t>
+  </si>
+  <si>
+    <t>... :- not study(X, computerscience), person(X).</t>
+  </si>
+  <si>
+    <t>... :- study_at(X, tuwien), person(X).</t>
+  </si>
+  <si>
+    <t>... :- not study_at(X, tuwien), person(X).</t>
+  </si>
+  <si>
+    <t>cNounVariableIsAdjectivePrepositioncNounVariable</t>
   </si>
 </sst>
 </file>
@@ -1148,8 +1222,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="99">
+  <cellStyleXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1265,7 +1353,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="99">
+  <cellStyles count="113">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1315,6 +1403,13 @@
     <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1364,6 +1459,13 @@
     <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1639,10 +1741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H65"/>
+  <dimension ref="A3:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" zoomScale="108" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="108" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1651,7 +1753,7 @@
     <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="47.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="39.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26.83203125" bestFit="1" customWidth="1"/>
@@ -1829,25 +1931,25 @@
         <v>7</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F10" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="H10" s="9" t="s">
         <v>258</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -1855,25 +1957,25 @@
         <v>8</v>
       </c>
       <c r="B11" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>277</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="E11" s="6" t="s">
+      <c r="F11" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="G11" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="H11" s="9" t="s">
         <v>262</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -1881,22 +1983,22 @@
         <v>9</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -1904,22 +2006,22 @@
         <v>10</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -1927,25 +2029,25 @@
         <v>11</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F14" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="H14" s="6" t="s">
         <v>258</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -1953,25 +2055,25 @@
         <v>12</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F15" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="H15" s="6" t="s">
         <v>262</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -1979,22 +2081,22 @@
         <v>13</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>28</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -2002,22 +2104,22 @@
         <v>14</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>28</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -2463,16 +2565,16 @@
         <v>232</v>
       </c>
       <c r="D36" t="s">
-        <v>237</v>
+        <v>296</v>
       </c>
       <c r="E36" t="s">
         <v>233</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -2486,16 +2588,16 @@
         <v>232</v>
       </c>
       <c r="D37" t="s">
-        <v>237</v>
+        <v>296</v>
       </c>
       <c r="E37" t="s">
         <v>234</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -2509,16 +2611,16 @@
         <v>232</v>
       </c>
       <c r="D38" t="s">
-        <v>237</v>
+        <v>296</v>
       </c>
       <c r="E38" t="s">
         <v>235</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
@@ -2532,16 +2634,16 @@
         <v>232</v>
       </c>
       <c r="D39" t="s">
-        <v>237</v>
+        <v>296</v>
       </c>
       <c r="E39" t="s">
         <v>236</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -2728,148 +2830,142 @@
         <v>123</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48">
+    <row r="48" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="6">
         <v>45</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D48" t="s">
-        <v>89</v>
-      </c>
-      <c r="E48" t="s">
-        <v>87</v>
-      </c>
-      <c r="G48" t="s">
-        <v>84</v>
-      </c>
-      <c r="H48" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49">
+      <c r="B48" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="H48" s="6" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="6">
         <v>46</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D49" t="s">
-        <v>89</v>
-      </c>
-      <c r="E49" t="s">
-        <v>92</v>
-      </c>
-      <c r="G49" t="s">
-        <v>93</v>
-      </c>
-      <c r="H49" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50">
+      <c r="B49" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="H49" s="6" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="6">
         <v>47</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D50" t="s">
-        <v>89</v>
-      </c>
-      <c r="E50" t="s">
-        <v>129</v>
-      </c>
-      <c r="G50" t="s">
-        <v>133</v>
-      </c>
-      <c r="H50" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51">
+      <c r="B50" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="H50" s="6" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="6">
         <v>48</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D51" t="s">
-        <v>89</v>
-      </c>
-      <c r="E51" t="s">
-        <v>130</v>
-      </c>
-      <c r="G51" t="s">
-        <v>134</v>
-      </c>
-      <c r="H51" t="s">
-        <v>132</v>
+      <c r="B51" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="H51" s="6" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>49</v>
       </c>
-      <c r="B52" t="s">
-        <v>96</v>
+      <c r="B52" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D52" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="E52" t="s">
-        <v>100</v>
-      </c>
-      <c r="F52" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="G52" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="H52" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>50</v>
       </c>
-      <c r="B53" t="s">
-        <v>97</v>
+      <c r="B53" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D53" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="E53" t="s">
-        <v>101</v>
-      </c>
-      <c r="F53" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="G53" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="H53" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
@@ -2877,25 +2973,22 @@
         <v>51</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D54" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="E54" t="s">
-        <v>108</v>
-      </c>
-      <c r="F54" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="G54" t="s">
-        <v>110</v>
+        <v>133</v>
       </c>
       <c r="H54" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
@@ -2903,25 +2996,22 @@
         <v>52</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D55" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="E55" t="s">
-        <v>114</v>
-      </c>
-      <c r="F55" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="G55" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="H55" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
@@ -2929,45 +3019,51 @@
         <v>53</v>
       </c>
       <c r="B56" t="s">
-        <v>147</v>
+        <v>96</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>145</v>
+        <v>98</v>
       </c>
       <c r="D56" t="s">
-        <v>146</v>
+        <v>99</v>
       </c>
       <c r="E56" t="s">
-        <v>149</v>
+        <v>100</v>
+      </c>
+      <c r="F56" t="s">
+        <v>102</v>
       </c>
       <c r="G56" t="s">
-        <v>153</v>
+        <v>103</v>
       </c>
       <c r="H56" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>54</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>148</v>
+      <c r="B57" t="s">
+        <v>97</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>145</v>
+        <v>98</v>
       </c>
       <c r="D57" t="s">
-        <v>146</v>
+        <v>99</v>
       </c>
       <c r="E57" t="s">
-        <v>150</v>
+        <v>101</v>
+      </c>
+      <c r="F57" t="s">
+        <v>105</v>
       </c>
       <c r="G57" t="s">
-        <v>152</v>
+        <v>106</v>
       </c>
       <c r="H57" t="s">
-        <v>151</v>
+        <v>107</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
@@ -2975,19 +3071,25 @@
         <v>55</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>157</v>
+        <v>115</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>156</v>
+        <v>98</v>
       </c>
       <c r="D58" t="s">
-        <v>155</v>
+        <v>99</v>
       </c>
       <c r="E58" t="s">
-        <v>159</v>
-      </c>
-      <c r="G58" s="5" t="s">
-        <v>154</v>
+        <v>108</v>
+      </c>
+      <c r="F58" t="s">
+        <v>109</v>
+      </c>
+      <c r="G58" t="s">
+        <v>110</v>
+      </c>
+      <c r="H58" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
@@ -2995,42 +3097,48 @@
         <v>56</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>158</v>
+        <v>116</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>156</v>
+        <v>98</v>
       </c>
       <c r="D59" t="s">
-        <v>155</v>
+        <v>99</v>
       </c>
       <c r="E59" t="s">
-        <v>161</v>
+        <v>114</v>
+      </c>
+      <c r="F59" t="s">
+        <v>112</v>
       </c>
       <c r="G59" t="s">
-        <v>160</v>
+        <v>113</v>
+      </c>
+      <c r="H59" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>57</v>
       </c>
-      <c r="B60" s="2" t="s">
-        <v>164</v>
+      <c r="B60" t="s">
+        <v>147</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="D60" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="E60" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="G60" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="H60" t="s">
-        <v>166</v>
+        <v>36</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
@@ -3038,35 +3146,121 @@
         <v>58</v>
       </c>
       <c r="B61" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D61" t="s">
+        <v>146</v>
+      </c>
+      <c r="E61" t="s">
+        <v>150</v>
+      </c>
+      <c r="G61" t="s">
+        <v>152</v>
+      </c>
+      <c r="H61" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>59</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D62" t="s">
+        <v>155</v>
+      </c>
+      <c r="E62" t="s">
+        <v>159</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>60</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D63" t="s">
+        <v>155</v>
+      </c>
+      <c r="E63" t="s">
+        <v>161</v>
+      </c>
+      <c r="G63" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>61</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D64" t="s">
+        <v>163</v>
+      </c>
+      <c r="E64" t="s">
+        <v>167</v>
+      </c>
+      <c r="G64" t="s">
+        <v>170</v>
+      </c>
+      <c r="H64" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>62</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C65" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D65" t="s">
         <v>163</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E65" t="s">
         <v>168</v>
       </c>
-      <c r="G61" t="s">
+      <c r="G65" t="s">
         <v>169</v>
       </c>
-      <c r="H61" s="5" t="s">
+      <c r="H65" s="5" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B62" s="2"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B63" s="2"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B64" s="2"/>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B65" s="2"/>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B66" s="2"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B67" s="2"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B68" s="2"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B69" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
gui: added sentence patterns
</commit_message>
<xml_diff>
--- a/sentences.xlsx
+++ b/sentences.xlsx
@@ -2,19 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
-  <workbookPr/>
+  <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiaskain/Google Drive/TU/6.Semester SS17/Bachelorarbeit/CNL/cnl2asp/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
+  <webPublishing allowPng="1" targetScreenSize="1024x768" codePage="10000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="331">
   <si>
     <t>Structure</t>
   </si>
@@ -1138,6 +1140,168 @@
   </si>
   <si>
     <t>cNounVariableIsAdjectivePrepositioncNounVariable</t>
+  </si>
+  <si>
+    <t>pNounIsCNounOfCNounVariable</t>
+  </si>
+  <si>
+    <t>Bob is the father of person X.</t>
+  </si>
+  <si>
+    <t>father(bob, X) :- ...</t>
+  </si>
+  <si>
+    <t>Bob is not the father of person X.</t>
+  </si>
+  <si>
+    <t>PNoun is not [the] CNoun of [a] CNoun Variable.</t>
+  </si>
+  <si>
+    <t>PNoun is [the] CNoun of [a] CNoun Variable.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - father(bob, X) :- ...</t>
+  </si>
+  <si>
+    <t>... :- father(bob, X), person(X).</t>
+  </si>
+  <si>
+    <t>... :- not father(bob, X), person(X).</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">.* is(n't | n't | not | ).* of .* [a-z] </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+      </rPr>
+      <t>\\</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>[a] CNoun Variable is not [the] CNoun of [a] PNoun.</t>
+  </si>
+  <si>
+    <t>[a] CNoun Variable is [the] CNoun of [a] PNoun.</t>
+  </si>
+  <si>
+    <r>
+      <t>.* [a-z] is(n't | n't | not | ).* of .*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+      </rPr>
+      <t>\\</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>cNounVariableIsCNounOfPNoun</t>
+  </si>
+  <si>
+    <t>Person X is the father of bob.</t>
+  </si>
+  <si>
+    <t>Person X is not the father of bob.</t>
+  </si>
+  <si>
+    <t>father(X, bob) :- ...</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - father(X, bob) :- ...</t>
+  </si>
+  <si>
+    <t>... :- father(X, bob), person(X).</t>
+  </si>
+  <si>
+    <t>... :- not father(X, bob), person(X).</t>
+  </si>
+  <si>
+    <t>PNoun is [the] CNoun of [a] PNoun.</t>
+  </si>
+  <si>
+    <t>PNoun is not [the] CNoun of [a] PNoun.</t>
+  </si>
+  <si>
+    <r>
+      <t>.* is(n't | n't | not | ).* of .*</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+      </rPr>
+      <t>\\</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>pNounIsCNounOfPNoun</t>
+  </si>
+  <si>
+    <t>Bob is the father of roberta.</t>
+  </si>
+  <si>
+    <t>Bob is not the father of roberta.</t>
+  </si>
+  <si>
+    <t>father(bob, roberta) :- ...</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - father(bob, roberta) :- ...</t>
+  </si>
+  <si>
+    <t>father(bob, roberta).</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - father(bob, roberta).</t>
+  </si>
+  <si>
+    <t>... :- father(bob, roberta).</t>
+  </si>
+  <si>
+    <t>... :- not father(bob, roberta).</t>
+  </si>
+  <si>
+    <t>Nr.</t>
+  </si>
+  <si>
+    <t>asdfasldkfjöalksdfjölajksd</t>
   </si>
 </sst>
 </file>
@@ -1204,7 +1368,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1221,8 +1385,76 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="113">
+  <cellStyleXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1336,8 +1568,26 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1352,8 +1602,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="113">
+  <cellStyles count="131">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1410,6 +1675,15 @@
     <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1466,6 +1740,15 @@
     <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1741,10 +2024,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H69"/>
+  <dimension ref="A3:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="108" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView showRuler="0" zoomScale="108" workbookViewId="0">
+      <selection activeCell="B25" sqref="A3:H71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3251,16 +3534,1013 @@
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B66" s="2"/>
+      <c r="A66">
+        <v>63</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="E66" t="s">
+        <v>298</v>
+      </c>
+      <c r="G66" t="s">
+        <v>304</v>
+      </c>
+      <c r="H66" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B67" s="2"/>
+      <c r="A67">
+        <v>64</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="E67" t="s">
+        <v>300</v>
+      </c>
+      <c r="G67" t="s">
+        <v>305</v>
+      </c>
+      <c r="H67" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B68" s="2"/>
+      <c r="A68">
+        <v>65</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="D68" t="s">
+        <v>310</v>
+      </c>
+      <c r="E68" t="s">
+        <v>311</v>
+      </c>
+      <c r="G68" t="s">
+        <v>315</v>
+      </c>
+      <c r="H68" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B69" s="2"/>
+      <c r="A69">
+        <v>66</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="D69" t="s">
+        <v>310</v>
+      </c>
+      <c r="E69" t="s">
+        <v>312</v>
+      </c>
+      <c r="G69" t="s">
+        <v>316</v>
+      </c>
+      <c r="H69" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>67</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D70" t="s">
+        <v>320</v>
+      </c>
+      <c r="E70" t="s">
+        <v>321</v>
+      </c>
+      <c r="F70" t="s">
+        <v>325</v>
+      </c>
+      <c r="G70" t="s">
+        <v>327</v>
+      </c>
+      <c r="H70" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>68</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D71" t="s">
+        <v>320</v>
+      </c>
+      <c r="E71" t="s">
+        <v>322</v>
+      </c>
+      <c r="F71" t="s">
+        <v>326</v>
+      </c>
+      <c r="G71" t="s">
+        <v>328</v>
+      </c>
+      <c r="H71" t="s">
+        <v>324</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H72"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="55.33203125" customWidth="1"/>
+    <col min="3" max="3" width="40.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>329</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+    </row>
+    <row r="2" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+    </row>
+    <row r="3" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15">
+        <v>2</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
+        <v>3</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="15">
+        <v>4</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15">
+        <v>5</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15">
+        <v>6</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15">
+        <v>7</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>253</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="9"/>
+    </row>
+    <row r="9" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15">
+        <v>8</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>260</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="9"/>
+    </row>
+    <row r="10" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15">
+        <v>9</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>248</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15">
+        <v>10</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>269</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15">
+        <v>11</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
+        <v>12</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>272</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15">
+        <v>13</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>256</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>273</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15">
+        <v>15</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15">
+        <v>16</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15">
+        <v>17</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="15">
+        <v>18</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="15">
+        <v>19</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="15">
+        <v>20</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="15">
+        <v>21</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="15">
+        <v>22</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="15">
+        <v>23</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="15">
+        <v>24</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="15">
+        <v>25</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="15">
+        <v>26</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="15">
+        <v>27</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="15">
+        <v>28</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+    </row>
+    <row r="30" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="15">
+        <v>29</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+    </row>
+    <row r="31" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="15">
+        <v>30</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+    </row>
+    <row r="32" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="15">
+        <v>31</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+    </row>
+    <row r="33" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="15">
+        <v>32</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+    </row>
+    <row r="34" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="15">
+        <v>33</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+    </row>
+    <row r="35" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="15">
+        <v>34</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+    </row>
+    <row r="36" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="15">
+        <v>35</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+    </row>
+    <row r="37" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="15">
+        <v>36</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+    </row>
+    <row r="38" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="15">
+        <v>37</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="15">
+        <v>38</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="15">
+        <v>39</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="15">
+        <v>40</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="15">
+        <v>41</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="15">
+        <v>42</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="15">
+        <v>43</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="15">
+        <v>44</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="15">
+        <v>45</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>280</v>
+      </c>
+      <c r="C46" s="16" t="s">
+        <v>284</v>
+      </c>
+      <c r="D46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+    </row>
+    <row r="47" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="15">
+        <v>46</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>283</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>285</v>
+      </c>
+      <c r="D47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+    </row>
+    <row r="48" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="15">
+        <v>47</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>281</v>
+      </c>
+      <c r="C48" s="16" t="s">
+        <v>286</v>
+      </c>
+      <c r="D48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+    </row>
+    <row r="49" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="15">
+        <v>48</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>282</v>
+      </c>
+      <c r="C49" s="16" t="s">
+        <v>287</v>
+      </c>
+      <c r="D49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+    </row>
+    <row r="50" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="15">
+        <v>49</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="15">
+        <v>50</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C51" s="16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="15">
+        <v>51</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="C52" s="16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="15">
+        <v>52</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="C53" s="16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="15">
+        <v>53</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C54" s="16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="15">
+        <v>54</v>
+      </c>
+      <c r="B55" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C55" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="15">
+        <v>55</v>
+      </c>
+      <c r="B56" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C56" s="16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="15">
+        <v>56</v>
+      </c>
+      <c r="B57" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="C57" s="16" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="15">
+        <v>57</v>
+      </c>
+      <c r="B58" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="C58" s="16" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="15">
+        <v>58</v>
+      </c>
+      <c r="B59" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="C59" s="16" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="15">
+        <v>59</v>
+      </c>
+      <c r="B60" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="C60" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="G60" s="5"/>
+    </row>
+    <row r="61" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="15">
+        <v>60</v>
+      </c>
+      <c r="B61" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C61" s="16" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="15">
+        <v>61</v>
+      </c>
+      <c r="B62" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="C62" s="16" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="15">
+        <v>62</v>
+      </c>
+      <c r="B63" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="C63" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="H63" s="5"/>
+    </row>
+    <row r="64" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="15">
+        <v>63</v>
+      </c>
+      <c r="B64" s="16" t="s">
+        <v>302</v>
+      </c>
+      <c r="C64" s="16" t="s">
+        <v>298</v>
+      </c>
+      <c r="D64" s="2"/>
+    </row>
+    <row r="65" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="15">
+        <v>64</v>
+      </c>
+      <c r="B65" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="C65" s="16" t="s">
+        <v>300</v>
+      </c>
+      <c r="D65" s="2"/>
+    </row>
+    <row r="66" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="15">
+        <v>65</v>
+      </c>
+      <c r="B66" s="16" t="s">
+        <v>308</v>
+      </c>
+      <c r="C66" s="16" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="15">
+        <v>66</v>
+      </c>
+      <c r="B67" s="16" t="s">
+        <v>307</v>
+      </c>
+      <c r="C67" s="16" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="15">
+        <v>67</v>
+      </c>
+      <c r="B68" s="16" t="s">
+        <v>317</v>
+      </c>
+      <c r="C68" s="16" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="15">
+        <v>68</v>
+      </c>
+      <c r="B69" s="16" t="s">
+        <v>318</v>
+      </c>
+      <c r="C69" s="16" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B72" t="s">
+        <v>330</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
replaced TextArea with RichTextFX
</commit_message>
<xml_diff>
--- a/sentences.xlsx
+++ b/sentences.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="448">
   <si>
     <t>Structure</t>
   </si>
@@ -1744,6 +1744,51 @@
   </si>
   <si>
     <t>Categorical Proposition Sentences</t>
+  </si>
+  <si>
+    <t>A CNoun Variable is a CNoun of a Cnoun Variable.</t>
+  </si>
+  <si>
+    <t>A CNoun Variable is not a CNoun of a CNoun Variable.</t>
+  </si>
+  <si>
+    <t>[A] CNoun Variable is [the] CNoun of [a] PNoun.</t>
+  </si>
+  <si>
+    <t>[A] CNoun Variable is not [the] CNoun of [a] PNoun.</t>
+  </si>
+  <si>
+    <t>There is a CNoun Variable.</t>
+  </si>
+  <si>
+    <t>There is not a CNoun Variable.</t>
+  </si>
+  <si>
+    <t>[A] CNoun Variable Verb a CNoun as [a] Pnoun.</t>
+  </si>
+  <si>
+    <t>[A] CNoun Variable not Verb a CNoun as [a] Pnoun.</t>
+  </si>
+  <si>
+    <t>[A] CNoun Variable Verb [a] CNoun Variable.</t>
+  </si>
+  <si>
+    <t>[A] CNoun Variable not Verb [a] CNoun Variable.</t>
+  </si>
+  <si>
+    <t>[A] CNoun Variable Verb Preposition [a] CNoun Variable.</t>
+  </si>
+  <si>
+    <t>[A] CNoun Variable not Verb Preposition [a] CNoun Variable.</t>
+  </si>
+  <si>
+    <t>[A] PNoun Verb a CNoun as [a] Pnoun.</t>
+  </si>
+  <si>
+    <t>[A] Pnoun not Verb a CNoun as [a] Pnoun.</t>
+  </si>
+  <si>
+    <t>PNoun not Verb.</t>
   </si>
 </sst>
 </file>
@@ -2189,10 +2234,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2709,8 +2754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:I92"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A63" zoomScale="108" workbookViewId="0">
-      <selection activeCell="E85" sqref="E85:E92"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="108" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2927,7 +2972,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>258</v>
+        <v>447</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>275</v>
@@ -3621,7 +3666,7 @@
         <v>37</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>136</v>
+        <v>445</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>140</v>
@@ -3644,7 +3689,7 @@
         <v>38</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>137</v>
+        <v>446</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>140</v>
@@ -3667,7 +3712,7 @@
         <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>71</v>
+        <v>439</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>68</v>
@@ -3690,7 +3735,7 @@
         <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>72</v>
+        <v>440</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>68</v>
@@ -3713,7 +3758,7 @@
         <v>41</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>119</v>
+        <v>441</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>77</v>
@@ -3736,7 +3781,7 @@
         <v>42</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>83</v>
+        <v>442</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>77</v>
@@ -3759,7 +3804,7 @@
         <v>43</v>
       </c>
       <c r="B46" t="s">
-        <v>118</v>
+        <v>443</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>77</v>
@@ -3782,7 +3827,7 @@
         <v>44</v>
       </c>
       <c r="B47" t="s">
-        <v>117</v>
+        <v>444</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>77</v>
@@ -4093,7 +4138,7 @@
         <v>57</v>
       </c>
       <c r="B60" t="s">
-        <v>147</v>
+        <v>437</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>145</v>
@@ -4116,7 +4161,7 @@
         <v>58</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>148</v>
+        <v>438</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>145</v>
@@ -4179,7 +4224,7 @@
         <v>61</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>163</v>
+        <v>433</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>372</v>
@@ -4202,7 +4247,7 @@
         <v>62</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>164</v>
+        <v>434</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>372</v>
@@ -4271,7 +4316,7 @@
         <v>65</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>306</v>
+        <v>435</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>374</v>
@@ -4294,7 +4339,7 @@
         <v>66</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>305</v>
+        <v>436</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>374</v>
@@ -4985,10 +5030,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H93"/>
+  <dimension ref="A1:H92"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="H96" sqref="H96"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="C71" sqref="C4:C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5006,9 +5051,9 @@
       <c r="C1" s="22"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
     </row>
     <row r="3" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
@@ -5857,225 +5902,214 @@
         <v>326</v>
       </c>
       <c r="C72" s="16" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="15">
-        <v>68</v>
-      </c>
-      <c r="B73" s="16" t="s">
-        <v>328</v>
-      </c>
-      <c r="C73" s="16" t="s">
-        <v>328</v>
-      </c>
+        <v>327</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="20" t="s">
+        <v>342</v>
+      </c>
+      <c r="B73" s="20"/>
+      <c r="C73" s="20"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="21" t="s">
-        <v>342</v>
-      </c>
+      <c r="A74" s="21"/>
       <c r="B74" s="21"/>
       <c r="C74" s="21"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="20"/>
-      <c r="B75" s="20"/>
-      <c r="C75" s="20"/>
-    </row>
-    <row r="76" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="17" t="s">
+    <row r="75" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="17" t="s">
         <v>325</v>
       </c>
-      <c r="B76" s="18" t="s">
+      <c r="B75" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C76" s="18" t="s">
+      <c r="C75" s="18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="15">
+        <v>69</v>
+      </c>
+      <c r="B76" s="16" t="s">
+        <v>330</v>
+      </c>
+      <c r="C76" s="16" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A77" s="15">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B77" s="16" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C77" s="16" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A78" s="15">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B78" s="16" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="C78" s="16" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="15">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B79" s="16" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="C79" s="16" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A80" s="15">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B80" s="16" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="C80" s="16" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A81" s="15">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B81" s="16" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="C81" s="16" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="15">
-        <v>74</v>
-      </c>
-      <c r="B82" s="16" t="s">
-        <v>340</v>
-      </c>
-      <c r="C82" s="16" t="s">
         <v>341</v>
       </c>
     </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="20" t="s">
+        <v>432</v>
+      </c>
+      <c r="B82" s="20"/>
+      <c r="C82" s="20"/>
+    </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83" s="21" t="s">
-        <v>432</v>
-      </c>
+      <c r="A83" s="21"/>
       <c r="B83" s="21"/>
       <c r="C83" s="21"/>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84" s="20"/>
-      <c r="B84" s="20"/>
-      <c r="C84" s="20"/>
-    </row>
-    <row r="85" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="17" t="s">
+    <row r="84" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="17" t="s">
         <v>325</v>
       </c>
-      <c r="B85" s="18" t="s">
+      <c r="B84" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C85" s="18" t="s">
+      <c r="C84" s="18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="15">
+        <v>75</v>
+      </c>
+      <c r="B85" s="16" t="s">
+        <v>366</v>
+      </c>
+      <c r="C85" s="16" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A86" s="15">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B86" s="16" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C86" s="16" t="s">
-        <v>394</v>
+        <v>361</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A87" s="15">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B87" s="16" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C87" s="16" t="s">
-        <v>361</v>
+        <v>399</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A88" s="15">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B88" s="16" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C88" s="16" t="s">
-        <v>399</v>
+        <v>362</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A89" s="15">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B89" s="16" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C89" s="16" t="s">
-        <v>362</v>
+        <v>407</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A90" s="15">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B90" s="16" t="s">
-        <v>370</v>
+        <v>387</v>
       </c>
       <c r="C90" s="16" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A91" s="15">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B91" s="16" t="s">
-        <v>387</v>
+        <v>371</v>
       </c>
       <c r="C91" s="16" t="s">
-        <v>408</v>
+        <v>363</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A92" s="15">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B92" s="16" t="s">
-        <v>371</v>
+        <v>388</v>
       </c>
       <c r="C92" s="16" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="15">
-        <v>82</v>
-      </c>
-      <c r="B93" s="16" t="s">
-        <v>388</v>
-      </c>
-      <c r="C93" s="16" t="s">
         <v>404</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A74:C75"/>
+    <mergeCell ref="A73:C74"/>
     <mergeCell ref="A1:C2"/>
-    <mergeCell ref="A83:C84"/>
+    <mergeCell ref="A82:C83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
display when translation is running
</commit_message>
<xml_diff>
--- a/sentences.xlsx
+++ b/sentences.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1873,7 +1873,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1890,85 +1890,8 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="233">
+  <cellStyleXfs count="237">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2202,8 +2125,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2221,30 +2148,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="233">
+  <cellStyles count="237">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2361,6 +2276,8 @@
     <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2477,6 +2394,8 @@
     <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2754,8 +2673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:I92"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="108" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView showRuler="0" topLeftCell="A67" zoomScale="108" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:E92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4722,7 +4641,7 @@
   </cols>
   <sheetData>
     <row r="7" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="13" t="s">
         <v>353</v>
       </c>
       <c r="C7" t="s">
@@ -4736,7 +4655,7 @@
       </c>
     </row>
     <row r="8" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="13" t="s">
         <v>354</v>
       </c>
       <c r="C8" t="s">
@@ -4750,7 +4669,7 @@
       </c>
     </row>
     <row r="9" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="13" t="s">
         <v>355</v>
       </c>
       <c r="D9" t="s">
@@ -4761,7 +4680,7 @@
       </c>
     </row>
     <row r="10" spans="2:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="13" t="s">
         <v>356</v>
       </c>
       <c r="D10" t="s">
@@ -5032,8 +4951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H92"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C71" sqref="C4:C71"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection sqref="A1:C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5044,25 +4963,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="14" t="s">
         <v>431</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-    </row>
-    <row r="3" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
         <v>325</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="10" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="10"/>
@@ -5070,14 +4989,14 @@
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
     </row>
-    <row r="4" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="16">
         <v>1</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="12"/>
@@ -5086,69 +5005,69 @@
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
     </row>
-    <row r="5" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="16">
         <v>2</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="16">
         <v>3</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="16">
         <v>4</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="16">
         <v>5</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="16">
         <v>6</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="15">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="16">
         <v>7</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="12" t="s">
         <v>252</v>
       </c>
       <c r="D10" s="6"/>
@@ -5156,14 +5075,14 @@
       <c r="G10" s="6"/>
       <c r="H10" s="9"/>
     </row>
-    <row r="11" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="16">
         <v>8</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="12" t="s">
         <v>258</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="12" t="s">
         <v>259</v>
       </c>
       <c r="D11" s="6"/>
@@ -5171,14 +5090,14 @@
       <c r="G11" s="6"/>
       <c r="H11" s="9"/>
     </row>
-    <row r="12" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="16">
         <v>9</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="12" t="s">
         <v>247</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="12" t="s">
         <v>253</v>
       </c>
       <c r="D12" s="6"/>
@@ -5186,14 +5105,14 @@
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
     </row>
-    <row r="13" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="16">
         <v>10</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="12" t="s">
         <v>270</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="12" t="s">
         <v>268</v>
       </c>
       <c r="D13" s="6"/>
@@ -5201,14 +5120,14 @@
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
     </row>
-    <row r="14" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="15">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="16">
         <v>11</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="12" t="s">
         <v>244</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="12" t="s">
         <v>254</v>
       </c>
       <c r="D14" s="6"/>
@@ -5216,14 +5135,14 @@
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="16">
         <v>12</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="12" t="s">
         <v>271</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="12" t="s">
         <v>269</v>
       </c>
       <c r="D15" s="6"/>
@@ -5231,14 +5150,14 @@
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
     </row>
-    <row r="16" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="15">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="16">
         <v>13</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="12" t="s">
         <v>245</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="12" t="s">
         <v>255</v>
       </c>
       <c r="D16" s="7"/>
@@ -5246,14 +5165,14 @@
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
     </row>
-    <row r="17" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="16">
         <v>14</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="12" t="s">
         <v>272</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="12" t="s">
         <v>276</v>
       </c>
       <c r="D17" s="7"/>
@@ -5261,363 +5180,363 @@
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
     </row>
-    <row r="18" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="15">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="16">
         <v>15</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="15">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="16">
         <v>16</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="15">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="16">
         <v>17</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="12" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="15">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="16">
         <v>18</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="12" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="15">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="16">
         <v>19</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="15">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="16">
         <v>20</v>
       </c>
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="15">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="16">
         <v>21</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="12" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="15">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="16">
         <v>22</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C25" s="12" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="15">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="16">
         <v>23</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="C26" s="12" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="15">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="16">
         <v>24</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="12" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="15">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="16">
         <v>25</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="12" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="15">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="16">
         <v>26</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="12" t="s">
         <v>207</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="C29" s="12" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="15">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="16">
         <v>27</v>
       </c>
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="C30" s="16" t="s">
+      <c r="C30" s="12" t="s">
         <v>190</v>
       </c>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="15">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="16">
         <v>28</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="12" t="s">
         <v>209</v>
       </c>
-      <c r="C31" s="16" t="s">
+      <c r="C31" s="12" t="s">
         <v>191</v>
       </c>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
     </row>
-    <row r="32" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="15">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="16">
         <v>29</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="12" t="s">
         <v>213</v>
       </c>
-      <c r="C32" s="16" t="s">
+      <c r="C32" s="12" t="s">
         <v>220</v>
       </c>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
     </row>
-    <row r="33" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="15">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="16">
         <v>30</v>
       </c>
-      <c r="B33" s="16" t="s">
+      <c r="B33" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="C33" s="16" t="s">
+      <c r="C33" s="12" t="s">
         <v>221</v>
       </c>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
     </row>
-    <row r="34" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="15">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="16">
         <v>31</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="12" t="s">
         <v>218</v>
       </c>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
     </row>
-    <row r="35" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="15">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="16">
         <v>32</v>
       </c>
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="C35" s="16" t="s">
+      <c r="C35" s="12" t="s">
         <v>219</v>
       </c>
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
     </row>
-    <row r="36" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="15">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="16">
         <v>33</v>
       </c>
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="C36" s="16" t="s">
+      <c r="C36" s="12" t="s">
         <v>232</v>
       </c>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
     </row>
-    <row r="37" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="15">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="16">
         <v>34</v>
       </c>
-      <c r="B37" s="16" t="s">
+      <c r="B37" s="12" t="s">
         <v>210</v>
       </c>
-      <c r="C37" s="16" t="s">
+      <c r="C37" s="12" t="s">
         <v>233</v>
       </c>
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
     </row>
-    <row r="38" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="15">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="16">
         <v>35</v>
       </c>
-      <c r="B38" s="16" t="s">
+      <c r="B38" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="C38" s="16" t="s">
+      <c r="C38" s="12" t="s">
         <v>234</v>
       </c>
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
     </row>
-    <row r="39" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="15">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="16">
         <v>36</v>
       </c>
-      <c r="B39" s="16" t="s">
+      <c r="B39" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="C39" s="16" t="s">
+      <c r="C39" s="12" t="s">
         <v>235</v>
       </c>
       <c r="G39" s="5"/>
       <c r="H39" s="5"/>
     </row>
-    <row r="40" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="15">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="16">
         <v>37</v>
       </c>
-      <c r="B40" s="16" t="s">
+      <c r="B40" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="C40" s="16" t="s">
+      <c r="C40" s="12" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="15">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="16">
         <v>38</v>
       </c>
-      <c r="B41" s="16" t="s">
+      <c r="B41" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="C41" s="16" t="s">
+      <c r="C41" s="12" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="15">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="16">
         <v>39</v>
       </c>
-      <c r="B42" s="16" t="s">
+      <c r="B42" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="C42" s="16" t="s">
+      <c r="C42" s="12" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="15">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="16">
         <v>40</v>
       </c>
-      <c r="B43" s="16" t="s">
+      <c r="B43" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C43" s="16" t="s">
+      <c r="C43" s="12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="15">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="16">
         <v>41</v>
       </c>
-      <c r="B44" s="16" t="s">
+      <c r="B44" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="C44" s="16" t="s">
+      <c r="C44" s="12" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="15">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="16">
         <v>42</v>
       </c>
-      <c r="B45" s="16" t="s">
+      <c r="B45" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="C45" s="16" t="s">
+      <c r="C45" s="12" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="15">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="16">
         <v>43</v>
       </c>
-      <c r="B46" s="16" t="s">
+      <c r="B46" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="C46" s="16" t="s">
+      <c r="C46" s="12" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="15">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="16">
         <v>44</v>
       </c>
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="C47" s="16" t="s">
+      <c r="C47" s="12" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="15">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="16">
         <v>45</v>
       </c>
-      <c r="B48" s="16" t="s">
+      <c r="B48" s="12" t="s">
         <v>279</v>
       </c>
-      <c r="C48" s="16" t="s">
+      <c r="C48" s="12" t="s">
         <v>283</v>
       </c>
       <c r="D48" s="6"/>
@@ -5625,14 +5544,14 @@
       <c r="G48" s="6"/>
       <c r="H48" s="6"/>
     </row>
-    <row r="49" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="15">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="16">
         <v>46</v>
       </c>
-      <c r="B49" s="16" t="s">
+      <c r="B49" s="12" t="s">
         <v>282</v>
       </c>
-      <c r="C49" s="16" t="s">
+      <c r="C49" s="12" t="s">
         <v>284</v>
       </c>
       <c r="D49" s="6"/>
@@ -5640,14 +5559,14 @@
       <c r="G49" s="6"/>
       <c r="H49" s="6"/>
     </row>
-    <row r="50" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="15">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="16">
         <v>47</v>
       </c>
-      <c r="B50" s="16" t="s">
+      <c r="B50" s="12" t="s">
         <v>280</v>
       </c>
-      <c r="C50" s="16" t="s">
+      <c r="C50" s="12" t="s">
         <v>285</v>
       </c>
       <c r="D50" s="6"/>
@@ -5655,14 +5574,14 @@
       <c r="G50" s="6"/>
       <c r="H50" s="6"/>
     </row>
-    <row r="51" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="15">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="16">
         <v>48</v>
       </c>
-      <c r="B51" s="16" t="s">
+      <c r="B51" s="12" t="s">
         <v>281</v>
       </c>
-      <c r="C51" s="16" t="s">
+      <c r="C51" s="12" t="s">
         <v>286</v>
       </c>
       <c r="D51" s="6"/>
@@ -5670,438 +5589,438 @@
       <c r="G51" s="6"/>
       <c r="H51" s="6"/>
     </row>
-    <row r="52" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="15">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="16">
         <v>49</v>
       </c>
-      <c r="B52" s="16" t="s">
+      <c r="B52" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="C52" s="16" t="s">
+      <c r="C52" s="12" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="15">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="16">
         <v>50</v>
       </c>
-      <c r="B53" s="16" t="s">
+      <c r="B53" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="C53" s="16" t="s">
+      <c r="C53" s="12" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="15">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="16">
         <v>51</v>
       </c>
-      <c r="B54" s="16" t="s">
+      <c r="B54" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="C54" s="16" t="s">
+      <c r="C54" s="12" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="15">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="16">
         <v>52</v>
       </c>
-      <c r="B55" s="16" t="s">
+      <c r="B55" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="C55" s="16" t="s">
+      <c r="C55" s="12" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="15">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="16">
         <v>53</v>
       </c>
-      <c r="B56" s="16" t="s">
+      <c r="B56" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="C56" s="16" t="s">
+      <c r="C56" s="12" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="15">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="16">
         <v>54</v>
       </c>
-      <c r="B57" s="16" t="s">
+      <c r="B57" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="C57" s="16" t="s">
+      <c r="C57" s="12" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="15">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="16">
         <v>55</v>
       </c>
-      <c r="B58" s="16" t="s">
+      <c r="B58" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="C58" s="16" t="s">
+      <c r="C58" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="15">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="16">
         <v>56</v>
       </c>
-      <c r="B59" s="16" t="s">
+      <c r="B59" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="C59" s="16" t="s">
+      <c r="C59" s="12" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="15">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="16">
         <v>57</v>
       </c>
-      <c r="B60" s="16" t="s">
+      <c r="B60" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="C60" s="16" t="s">
+      <c r="C60" s="12" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="15">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="16">
         <v>58</v>
       </c>
-      <c r="B61" s="16" t="s">
+      <c r="B61" s="12" t="s">
         <v>148</v>
       </c>
-      <c r="C61" s="16" t="s">
+      <c r="C61" s="12" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="15">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" s="16">
         <v>59</v>
       </c>
-      <c r="B62" s="16" t="s">
+      <c r="B62" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="C62" s="16" t="s">
+      <c r="C62" s="12" t="s">
         <v>159</v>
       </c>
       <c r="G62" s="5"/>
     </row>
-    <row r="63" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="15">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="16">
         <v>60</v>
       </c>
-      <c r="B63" s="16" t="s">
+      <c r="B63" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="C63" s="16" t="s">
+      <c r="C63" s="12" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="15">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="16">
         <v>61</v>
       </c>
-      <c r="B64" s="16" t="s">
+      <c r="B64" s="12" t="s">
         <v>163</v>
       </c>
-      <c r="C64" s="16" t="s">
+      <c r="C64" s="12" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="15">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" s="16">
         <v>62</v>
       </c>
-      <c r="B65" s="16" t="s">
+      <c r="B65" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="C65" s="16" t="s">
+      <c r="C65" s="12" t="s">
         <v>167</v>
       </c>
       <c r="H65" s="5"/>
     </row>
-    <row r="66" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="15">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="16">
         <v>63</v>
       </c>
-      <c r="B66" s="16" t="s">
+      <c r="B66" s="12" t="s">
         <v>301</v>
       </c>
-      <c r="C66" s="16" t="s">
+      <c r="C66" s="12" t="s">
         <v>297</v>
       </c>
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="15">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="16">
         <v>64</v>
       </c>
-      <c r="B67" s="16" t="s">
+      <c r="B67" s="12" t="s">
         <v>300</v>
       </c>
-      <c r="C67" s="16" t="s">
+      <c r="C67" s="12" t="s">
         <v>299</v>
       </c>
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="15">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="16">
         <v>65</v>
       </c>
-      <c r="B68" s="16" t="s">
+      <c r="B68" s="12" t="s">
         <v>306</v>
       </c>
-      <c r="C68" s="16" t="s">
+      <c r="C68" s="12" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="15">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" s="16">
         <v>66</v>
       </c>
-      <c r="B69" s="16" t="s">
+      <c r="B69" s="12" t="s">
         <v>305</v>
       </c>
-      <c r="C69" s="16" t="s">
+      <c r="C69" s="12" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="15">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" s="16">
         <v>67</v>
       </c>
-      <c r="B70" s="16" t="s">
+      <c r="B70" s="12" t="s">
         <v>314</v>
       </c>
-      <c r="C70" s="16" t="s">
+      <c r="C70" s="12" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="15">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" s="16">
         <v>68</v>
       </c>
-      <c r="B71" s="16" t="s">
+      <c r="B71" s="12" t="s">
         <v>315</v>
       </c>
-      <c r="C71" s="16" t="s">
+      <c r="C71" s="12" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="15">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" s="16">
         <v>68</v>
       </c>
-      <c r="B72" s="16" t="s">
+      <c r="B72" s="12" t="s">
         <v>326</v>
       </c>
-      <c r="C72" s="16" t="s">
+      <c r="C72" s="12" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" s="20" t="s">
+      <c r="A73" s="14" t="s">
         <v>342</v>
       </c>
-      <c r="B73" s="20"/>
-      <c r="C73" s="20"/>
+      <c r="B73" s="14"/>
+      <c r="C73" s="14"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="21"/>
-      <c r="B74" s="21"/>
-      <c r="C74" s="21"/>
-    </row>
-    <row r="75" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="17" t="s">
+      <c r="A74" s="14"/>
+      <c r="B74" s="14"/>
+      <c r="C74" s="14"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="15" t="s">
         <v>325</v>
       </c>
-      <c r="B75" s="18" t="s">
+      <c r="B75" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C75" s="18" t="s">
+      <c r="C75" s="10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="15">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" s="16">
         <v>69</v>
       </c>
-      <c r="B76" s="16" t="s">
+      <c r="B76" s="12" t="s">
         <v>330</v>
       </c>
-      <c r="C76" s="16" t="s">
+      <c r="C76" s="12" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="15">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" s="16">
         <v>70</v>
       </c>
-      <c r="B77" s="16" t="s">
+      <c r="B77" s="12" t="s">
         <v>332</v>
       </c>
-      <c r="C77" s="16" t="s">
+      <c r="C77" s="12" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="15">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" s="16">
         <v>71</v>
       </c>
-      <c r="B78" s="16" t="s">
+      <c r="B78" s="12" t="s">
         <v>334</v>
       </c>
-      <c r="C78" s="16" t="s">
+      <c r="C78" s="12" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="15">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" s="16">
         <v>72</v>
       </c>
-      <c r="B79" s="16" t="s">
+      <c r="B79" s="12" t="s">
         <v>336</v>
       </c>
-      <c r="C79" s="16" t="s">
+      <c r="C79" s="12" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="15">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" s="16">
         <v>73</v>
       </c>
-      <c r="B80" s="16" t="s">
+      <c r="B80" s="12" t="s">
         <v>338</v>
       </c>
-      <c r="C80" s="16" t="s">
+      <c r="C80" s="12" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="15">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="16">
         <v>74</v>
       </c>
-      <c r="B81" s="16" t="s">
+      <c r="B81" s="12" t="s">
         <v>340</v>
       </c>
-      <c r="C81" s="16" t="s">
+      <c r="C81" s="12" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" s="20" t="s">
+      <c r="A82" s="14" t="s">
         <v>432</v>
       </c>
-      <c r="B82" s="20"/>
-      <c r="C82" s="20"/>
+      <c r="B82" s="14"/>
+      <c r="C82" s="14"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83" s="21"/>
-      <c r="B83" s="21"/>
-      <c r="C83" s="21"/>
-    </row>
-    <row r="84" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="17" t="s">
+      <c r="A83" s="14"/>
+      <c r="B83" s="14"/>
+      <c r="C83" s="14"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="15" t="s">
         <v>325</v>
       </c>
-      <c r="B84" s="18" t="s">
+      <c r="B84" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C84" s="18" t="s">
+      <c r="C84" s="10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="15">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="16">
         <v>75</v>
       </c>
-      <c r="B85" s="16" t="s">
+      <c r="B85" s="12" t="s">
         <v>366</v>
       </c>
-      <c r="C85" s="16" t="s">
+      <c r="C85" s="12" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="15">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="16">
         <v>76</v>
       </c>
-      <c r="B86" s="16" t="s">
+      <c r="B86" s="12" t="s">
         <v>367</v>
       </c>
-      <c r="C86" s="16" t="s">
+      <c r="C86" s="12" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="15">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="16">
         <v>77</v>
       </c>
-      <c r="B87" s="16" t="s">
+      <c r="B87" s="12" t="s">
         <v>368</v>
       </c>
-      <c r="C87" s="16" t="s">
+      <c r="C87" s="12" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="15">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="16">
         <v>78</v>
       </c>
-      <c r="B88" s="16" t="s">
+      <c r="B88" s="12" t="s">
         <v>369</v>
       </c>
-      <c r="C88" s="16" t="s">
+      <c r="C88" s="12" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="15">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="16">
         <v>79</v>
       </c>
-      <c r="B89" s="16" t="s">
+      <c r="B89" s="12" t="s">
         <v>370</v>
       </c>
-      <c r="C89" s="16" t="s">
+      <c r="C89" s="12" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="15">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="16">
         <v>80</v>
       </c>
-      <c r="B90" s="16" t="s">
+      <c r="B90" s="12" t="s">
         <v>387</v>
       </c>
-      <c r="C90" s="16" t="s">
+      <c r="C90" s="12" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="15">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="16">
         <v>81</v>
       </c>
-      <c r="B91" s="16" t="s">
+      <c r="B91" s="12" t="s">
         <v>371</v>
       </c>
-      <c r="C91" s="16" t="s">
+      <c r="C91" s="12" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="15">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="16">
         <v>82</v>
       </c>
-      <c r="B92" s="16" t="s">
+      <c r="B92" s="12" t="s">
         <v>388</v>
       </c>
-      <c r="C92" s="16" t="s">
+      <c r="C92" s="12" t="s">
         <v>404</v>
       </c>
     </row>

</xml_diff>